<commit_message>
Added in more data to the excel sheet
</commit_message>
<xml_diff>
--- a/Capstone Project/Monika/Costs PerV3.xlsx
+++ b/Capstone Project/Monika/Costs PerV3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Desktop\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\Monika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF722AC-35FD-45FC-95C7-BF050F172BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ABF808-1784-48D5-A2E4-CDC35919F222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
   </bookViews>
@@ -92,15 +92,9 @@
     <t>Eletrical</t>
   </si>
   <si>
-    <t>Repairs 5% of Pop</t>
-  </si>
-  <si>
     <t>Population having cars</t>
   </si>
   <si>
-    <t>car owners</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -156,6 +150,12 @@
   </si>
   <si>
     <t>Population in BC</t>
+  </si>
+  <si>
+    <t>Precentage of Car Owners</t>
+  </si>
+  <si>
+    <t>% of Repairs</t>
   </si>
 </sst>
 </file>
@@ -165,7 +165,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -313,11 +313,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -643,13 +643,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6105DF2C-7430-48BF-A45E-C623D48AA4A1}">
   <dimension ref="A2:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.578125" customWidth="1"/>
+    <col min="1" max="1" width="30.89453125" customWidth="1"/>
     <col min="2" max="2" width="21.68359375" customWidth="1"/>
     <col min="3" max="3" width="15.7890625" customWidth="1"/>
     <col min="4" max="4" width="18.3125" customWidth="1"/>
@@ -680,7 +680,7 @@
   <sheetData>
     <row r="2" spans="1:36" ht="38.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -849,7 +849,7 @@
     </row>
     <row r="8" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -909,13 +909,13 @@
     </row>
     <row r="10" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="29">
-        <v>452500000</v>
+        <v>5070000</v>
       </c>
       <c r="B10" s="29">
-        <v>4213000</v>
+        <v>5010000</v>
       </c>
       <c r="C10" s="29">
-        <v>12345000</v>
+        <v>4920000</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -965,12 +965,12 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>19</v>
+    <row r="12" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A12" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="B12">
-        <v>5.0000000000000002E-5</v>
+        <v>1E-3</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -995,9 +995,9 @@
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>21</v>
+    <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A13" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="B13">
         <v>0.65</v>
@@ -1021,7 +1021,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1029,13 +1029,13 @@
       <c r="H15" s="1"/>
       <c r="I15" s="3"/>
       <c r="J15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="3"/>
       <c r="N15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1044,7 +1044,7 @@
       <c r="S15" s="15"/>
       <c r="T15" s="4"/>
       <c r="V15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -1065,13 +1065,13 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>16</v>
@@ -1089,7 +1089,7 @@
         <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>3</v>
@@ -1101,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>15</v>
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="T16" s="4" t="s">
         <v>14</v>
@@ -1174,256 +1174,253 @@
       </c>
       <c r="B17" s="11">
         <f>B24*0.3</f>
-        <v>88237500</v>
+        <v>988650</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="17">
-        <f>$B6 * (B17*B12)</f>
-        <v>5294250</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17">
         <f>$K6 * (B17*B12)</f>
-        <v>1941225</v>
+        <v>435006</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
         <f>$M6 * (B17*B12)</f>
-        <v>441187.5</v>
+        <v>98865</v>
       </c>
       <c r="I17" s="18">
         <f>SUM(D17:H17)</f>
-        <v>7676662.5</v>
+        <v>533871</v>
       </c>
       <c r="J17" s="17">
         <f>$D6 * (B17*B12)</f>
-        <v>352950</v>
+        <v>79092</v>
       </c>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="18">
-        <f>SUM(J17:L17)</f>
-        <v>352950</v>
+        <f t="shared" ref="M17:M23" si="0">SUM(J17:L17)</f>
+        <v>79092</v>
       </c>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
       <c r="P17" s="19">
         <f>$F6 * (B17*B12)</f>
-        <v>1411800</v>
+        <v>316368</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
       <c r="S17" s="20">
-        <f>SUM(N17:R17)</f>
-        <v>1411800</v>
+        <f t="shared" ref="S17:S23" si="1">SUM(N17:R17)</f>
+        <v>316368</v>
       </c>
       <c r="T17" s="21">
         <f>SUM(I17+M17)</f>
-        <v>8029612.5</v>
+        <v>612963</v>
       </c>
       <c r="V17" s="7">
         <f>A$6*4+(B17*B12)</f>
-        <v>5211.875</v>
+        <v>1788.65</v>
       </c>
       <c r="W17" s="7">
         <f>B$6*1+(B17*B12)</f>
-        <v>5611.875</v>
+        <v>2188.65</v>
       </c>
       <c r="X17" s="7">
         <f>C6*3++(B17*B12)</f>
-        <v>5011.875</v>
+        <v>1588.65</v>
       </c>
       <c r="Y17" s="7">
         <f>D6*2+(B17*B12)</f>
-        <v>4571.875</v>
+        <v>1148.6500000000001</v>
       </c>
       <c r="Z17" s="7">
         <f>E6*3+(B17*B12)</f>
-        <v>4771.875</v>
+        <v>1348.65</v>
       </c>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
       <c r="AC17" s="7">
         <f>H6*1+(B17*B12)</f>
-        <v>4511.875</v>
+        <v>1088.6500000000001</v>
       </c>
       <c r="AD17" s="7">
         <f>I6*1+(B17*B12)</f>
-        <v>5211.875</v>
+        <v>1788.65</v>
       </c>
       <c r="AE17" s="7"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="7"/>
       <c r="AH17" s="7">
         <f>M6*1+(B17*B12)</f>
-        <v>4511.875</v>
+        <v>1088.6500000000001</v>
       </c>
       <c r="AI17" s="5">
-        <f t="shared" ref="AI17:AI23" si="0">SUM(V17:AH17)</f>
-        <v>39415</v>
+        <f t="shared" ref="AI17:AI23" si="2">SUM(V17:AH17)</f>
+        <v>12029.199999999999</v>
       </c>
       <c r="AJ17" s="8">
-        <f t="shared" ref="AJ17:AJ23" si="1">SUM(I17+M17+AI17)</f>
-        <v>8069027.5</v>
+        <f t="shared" ref="AJ17:AJ23" si="3">SUM(I17+M17+AI17)</f>
+        <v>624992.19999999995</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2"/>
       <c r="B18" s="11">
         <f>B24*0.27</f>
-        <v>79413750</v>
+        <v>889785.00000000012</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" s="17">
         <f>$B6 * (B18*B12)</f>
-        <v>4764825</v>
+        <v>1067742</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="I18" s="18">
-        <f t="shared" ref="I18:I24" si="2">SUM(D18:H18)</f>
-        <v>4764825</v>
+        <f t="shared" ref="I18:I40" si="4">SUM(D18:H18)</f>
+        <v>1067742</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19">
         <f>$D6 * (B18*B12)</f>
-        <v>317655</v>
+        <v>71182.8</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="18">
-        <f>SUM(J18:L18)</f>
-        <v>317655</v>
+        <f t="shared" si="0"/>
+        <v>71182.8</v>
       </c>
       <c r="N18" s="19">
         <f>$A6 * (B18*B12)</f>
-        <v>794137.5</v>
+        <v>177957.00000000003</v>
       </c>
       <c r="O18" s="19"/>
       <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
       <c r="R18" s="19"/>
       <c r="S18" s="20">
-        <f>SUM(N18:R18)</f>
-        <v>794137.5</v>
+        <f t="shared" si="1"/>
+        <v>177957.00000000003</v>
       </c>
       <c r="T18" s="21">
-        <f t="shared" ref="T18:T24" si="3">SUM(I18+M18)</f>
-        <v>5082480</v>
+        <f t="shared" ref="T18:T24" si="5">SUM(I18+M18)</f>
+        <v>1138924.8</v>
       </c>
       <c r="V18" s="7">
         <f>A$6*1+(B18*B12)</f>
-        <v>4170.6875</v>
+        <v>1089.7850000000001</v>
       </c>
       <c r="W18" s="7">
         <f>B$6*1++(B18*B12)</f>
-        <v>5170.6875</v>
+        <v>2089.7849999999999</v>
       </c>
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7">
         <f>E6*2+(B18*B12)</f>
-        <v>4210.6875</v>
+        <v>1129.7850000000001</v>
       </c>
       <c r="AA18" s="7">
         <f>F6*1+(B18*B12)</f>
-        <v>4290.6875</v>
+        <v>1209.7850000000001</v>
       </c>
       <c r="AB18" s="7">
         <f>G6*1+(B18*B12)</f>
-        <v>4670.6875</v>
+        <v>1589.7850000000001</v>
       </c>
       <c r="AC18" s="7">
         <f>H6*1+(B18*B12)</f>
-        <v>4070.6875</v>
+        <v>989.78500000000008</v>
       </c>
       <c r="AD18" s="7"/>
       <c r="AE18" s="7"/>
       <c r="AF18" s="7"/>
       <c r="AG18" s="7">
         <f>L6*1+(B18*B12)</f>
-        <v>4170.6875</v>
+        <v>1089.7850000000001</v>
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="5">
-        <f t="shared" si="0"/>
-        <v>30754.8125</v>
+        <f t="shared" si="2"/>
+        <v>9188.494999999999</v>
       </c>
       <c r="AJ18" s="8">
-        <f t="shared" si="1"/>
-        <v>5113234.8125</v>
+        <f t="shared" si="3"/>
+        <v>1148113.2950000002</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2"/>
       <c r="B19" s="11">
         <f>B24*0.17</f>
-        <v>50001250</v>
+        <v>560235</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17">
         <f>$C6 * (B19*B12)</f>
-        <v>500012.5</v>
+        <v>112047</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
         <f>$M6 * (B19*B12)</f>
-        <v>250006.25</v>
+        <v>56023.5</v>
       </c>
       <c r="I19" s="18">
-        <f t="shared" si="2"/>
-        <v>750018.75</v>
+        <f t="shared" si="4"/>
+        <v>168070.5</v>
       </c>
       <c r="J19" s="19">
         <f>$D6 * (B19*B12)</f>
-        <v>200005</v>
+        <v>44818.8</v>
       </c>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18">
-        <f>SUM(J19:L19)</f>
-        <v>200005</v>
+        <f t="shared" si="0"/>
+        <v>44818.8</v>
       </c>
       <c r="N19" s="19"/>
       <c r="O19" s="19">
         <f>$E6 * (B19*B12)</f>
-        <v>300007.5</v>
+        <v>67228.2</v>
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
       <c r="S19" s="20">
-        <f>SUM(N19:R19)</f>
-        <v>300007.5</v>
+        <f t="shared" si="1"/>
+        <v>67228.2</v>
       </c>
       <c r="T19" s="21">
-        <f t="shared" si="3"/>
-        <v>950023.75</v>
+        <f t="shared" si="5"/>
+        <v>212889.3</v>
       </c>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
       <c r="Y19" s="7">
         <f>D6*1+(B19*B12)</f>
-        <v>2580.0625</v>
+        <v>640.23500000000001</v>
       </c>
       <c r="Z19" s="7">
         <f>E6*1+(B19*B12)</f>
-        <v>2620.0625</v>
+        <v>680.23500000000001</v>
       </c>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
       <c r="AC19" s="7">
         <f>H6*2+(B19*B12)</f>
-        <v>2700.0625</v>
+        <v>760.23500000000001</v>
       </c>
       <c r="AD19" s="7"/>
       <c r="AE19" s="7"/>
@@ -1431,141 +1428,141 @@
       <c r="AG19" s="7"/>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5">
-        <f t="shared" si="0"/>
-        <v>7900.1875</v>
+        <f t="shared" si="2"/>
+        <v>2080.7049999999999</v>
       </c>
       <c r="AJ19" s="8">
-        <f t="shared" si="1"/>
-        <v>957923.9375</v>
+        <f t="shared" si="3"/>
+        <v>214970.00499999998</v>
       </c>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2"/>
       <c r="B20" s="11">
         <f>B24*0.09</f>
-        <v>26471250</v>
+        <v>296595</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17">
         <f>$K6 * (B20*B12)</f>
-        <v>582367.5</v>
+        <v>130501.80000000002</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
       <c r="I20" s="18">
-        <f t="shared" si="2"/>
-        <v>582367.5</v>
+        <f t="shared" si="4"/>
+        <v>130501.80000000002</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19">
         <f>$D6 * (B20*B12)</f>
-        <v>105885</v>
+        <v>23727.600000000002</v>
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="18">
-        <f>SUM(J20:L20)</f>
-        <v>105885</v>
+        <f t="shared" si="0"/>
+        <v>23727.600000000002</v>
       </c>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
       <c r="P20" s="19"/>
       <c r="Q20" s="19">
         <f>$G6 * (B20*B12)</f>
-        <v>926493.75</v>
+        <v>207616.50000000003</v>
       </c>
       <c r="R20" s="19"/>
       <c r="S20" s="20">
-        <f>SUM(N20:R20)</f>
-        <v>926493.75</v>
+        <f t="shared" si="1"/>
+        <v>207616.50000000003</v>
       </c>
       <c r="T20" s="21">
-        <f t="shared" si="3"/>
-        <v>688252.5</v>
+        <f t="shared" si="5"/>
+        <v>154229.40000000002</v>
       </c>
       <c r="V20" s="7">
         <f>A6*1+(B20*B12)</f>
-        <v>1523.5625</v>
+        <v>496.59500000000003</v>
       </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7">
         <f>C6*1+(B20*B12)</f>
-        <v>1523.5625</v>
+        <v>496.59500000000003</v>
       </c>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="7"/>
       <c r="AB20" s="7">
         <f>G6*1+(B20*B12)</f>
-        <v>2023.5625</v>
+        <v>996.59500000000003</v>
       </c>
       <c r="AC20" s="7"/>
       <c r="AD20" s="7">
         <f>I6*1+(B20*B12)</f>
-        <v>2123.5625</v>
+        <v>1096.595</v>
       </c>
       <c r="AE20" s="7"/>
       <c r="AF20" s="7"/>
       <c r="AG20" s="7"/>
       <c r="AH20" s="7"/>
       <c r="AI20" s="5">
-        <f t="shared" si="0"/>
-        <v>7194.25</v>
+        <f t="shared" si="2"/>
+        <v>3086.38</v>
       </c>
       <c r="AJ20" s="8">
-        <f t="shared" si="1"/>
-        <v>695446.75</v>
+        <f t="shared" si="3"/>
+        <v>157315.78000000003</v>
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2"/>
       <c r="B21" s="11">
         <f>B24*0.07</f>
-        <v>20588750.000000004</v>
+        <v>230685.00000000003</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="17">
         <f>$B6 * (B21*B12)</f>
-        <v>1235325.0000000002</v>
+        <v>276822.00000000006</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17">
         <f>$L6 * (B20*B12)</f>
-        <v>264712.5</v>
+        <v>59319.000000000007</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="18">
-        <f t="shared" si="2"/>
-        <v>1500037.5000000002</v>
+        <f t="shared" si="4"/>
+        <v>336141.00000000006</v>
       </c>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="18">
-        <f>SUM(J21:L21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N21" s="19"/>
       <c r="O21" s="19">
         <f>$E6 * (B21*B12)</f>
-        <v>123532.50000000003</v>
+        <v>27682.200000000004</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
       <c r="S21" s="20">
-        <f>SUM(N21:R21)</f>
-        <v>123532.50000000003</v>
+        <f t="shared" si="1"/>
+        <v>27682.200000000004</v>
       </c>
       <c r="T21" s="21">
-        <f t="shared" si="3"/>
-        <v>1500037.5000000002</v>
+        <f t="shared" si="5"/>
+        <v>336141.00000000006</v>
       </c>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
@@ -1573,7 +1570,7 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7">
         <f>E6*1+(B21*B12)</f>
-        <v>1149.4375000000002</v>
+        <v>350.68500000000006</v>
       </c>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
@@ -1584,66 +1581,69 @@
       <c r="AG21" s="7"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="5">
-        <f t="shared" si="0"/>
-        <v>1149.4375000000002</v>
+        <f t="shared" si="2"/>
+        <v>350.68500000000006</v>
       </c>
       <c r="AJ21" s="8">
-        <f t="shared" si="1"/>
-        <v>1501186.9375000002</v>
+        <f t="shared" si="3"/>
+        <v>336491.68500000006</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2"/>
       <c r="B22" s="11">
         <f>B24*0.06</f>
-        <v>17647500</v>
+        <v>197730</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17">
         <f>$K6 * (B21*B12)</f>
-        <v>452952.50000000012</v>
+        <v>101501.40000000001</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="18">
-        <f t="shared" si="2"/>
-        <v>452952.50000000012</v>
-      </c>
-      <c r="J22" s="19"/>
+        <f t="shared" si="4"/>
+        <v>101501.40000000001</v>
+      </c>
+      <c r="J22" s="19">
+        <f>$D6 * (B22*B12)</f>
+        <v>15818.400000000001</v>
+      </c>
       <c r="K22" s="19"/>
       <c r="L22" s="19">
         <f>$J6 * (B22*B12)</f>
-        <v>238241.25</v>
+        <v>53387.100000000006</v>
       </c>
       <c r="M22" s="18">
-        <f>SUM(J22:L22)</f>
-        <v>238241.25</v>
+        <f t="shared" si="0"/>
+        <v>69205.5</v>
       </c>
       <c r="N22" s="19">
         <f>$A6 * (B22*B12)</f>
-        <v>176475</v>
+        <v>39546</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="19"/>
       <c r="S22" s="20">
-        <f>SUM(N22:R22)</f>
-        <v>176475</v>
+        <f t="shared" si="1"/>
+        <v>39546</v>
       </c>
       <c r="T22" s="21">
-        <f t="shared" si="3"/>
-        <v>691193.75000000012</v>
+        <f t="shared" si="5"/>
+        <v>170706.90000000002</v>
       </c>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="X22" s="7">
         <f>C6*1+(B22*B12)</f>
-        <v>1082.375</v>
+        <v>397.73</v>
       </c>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
@@ -1654,52 +1654,58 @@
       <c r="AE22" s="7"/>
       <c r="AF22" s="7">
         <f>K6*1+(B22*B12)</f>
-        <v>1322.375</v>
+        <v>637.73</v>
       </c>
       <c r="AG22" s="7"/>
       <c r="AH22" s="7">
         <f>M6*1+(B22*B12)</f>
-        <v>982.375</v>
+        <v>297.73</v>
       </c>
       <c r="AI22" s="5">
-        <f t="shared" si="0"/>
-        <v>3387.125</v>
+        <f t="shared" si="2"/>
+        <v>1333.19</v>
       </c>
       <c r="AJ22" s="8">
-        <f t="shared" si="1"/>
-        <v>694580.87500000012</v>
+        <f t="shared" si="3"/>
+        <v>172040.09000000003</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2"/>
       <c r="B23" s="11">
         <f>B24*0.04</f>
-        <v>11765000</v>
+        <v>131820</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17">
         <f>$C6 * (B23*B12)</f>
-        <v>117650</v>
-      </c>
-      <c r="F23" s="17"/>
+        <v>26364</v>
+      </c>
+      <c r="F23" s="17">
+        <f>$K6 * (B23*B12)</f>
+        <v>58000.799999999996</v>
+      </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
         <f>$M6 * (B23*B12)</f>
-        <v>58825</v>
+        <v>13182</v>
       </c>
       <c r="I23" s="18">
         <f>SUM(D23:H23)</f>
-        <v>176475</v>
+        <v>97546.799999999988</v>
       </c>
       <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="K23" s="19">
+        <f>$I6 * (B23*B12)</f>
+        <v>105456</v>
+      </c>
       <c r="L23" s="19"/>
       <c r="M23" s="18">
-        <f>SUM(J23:L23)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>105456</v>
       </c>
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
@@ -1707,15 +1713,15 @@
       <c r="Q23" s="19"/>
       <c r="R23" s="19">
         <f>$H6 * (B23*B12)</f>
-        <v>58825</v>
+        <v>13182</v>
       </c>
       <c r="S23" s="20">
-        <f>SUM(N23:R23)</f>
-        <v>58825</v>
+        <f t="shared" si="1"/>
+        <v>13182</v>
       </c>
       <c r="T23" s="21">
-        <f t="shared" si="3"/>
-        <v>176475</v>
+        <f t="shared" si="5"/>
+        <v>203002.8</v>
       </c>
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
@@ -1725,7 +1731,7 @@
       <c r="AA23" s="7"/>
       <c r="AB23" s="7">
         <f>G6*1+(B23*B12)</f>
-        <v>1288.25</v>
+        <v>831.81999999999994</v>
       </c>
       <c r="AC23" s="7"/>
       <c r="AD23" s="7"/>
@@ -1734,150 +1740,150 @@
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
       <c r="AI23" s="5">
-        <f t="shared" si="0"/>
-        <v>1288.25</v>
+        <f t="shared" si="2"/>
+        <v>831.81999999999994</v>
       </c>
       <c r="AJ23" s="8">
-        <f t="shared" si="1"/>
-        <v>177763.25</v>
+        <f t="shared" si="3"/>
+        <v>203834.62</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" s="9">
-        <f>452500000*B13</f>
-        <v>294125000</v>
+        <f>A10*B13</f>
+        <v>3295500</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="18">
         <f>SUM(D17:D23)</f>
-        <v>11294400</v>
+        <v>1344564</v>
       </c>
       <c r="E24" s="18">
         <f>SUM(E17:E23)</f>
-        <v>617662.5</v>
+        <v>138411</v>
       </c>
       <c r="F24" s="18">
         <f>SUM(F17:F23)</f>
-        <v>2523592.5</v>
+        <v>623508.60000000009</v>
       </c>
       <c r="G24" s="18">
         <f>SUM(G17:G23)</f>
-        <v>717665.00000000012</v>
+        <v>160820.40000000002</v>
       </c>
       <c r="H24" s="18">
         <f>SUM(H17:H23)</f>
-        <v>750018.75</v>
+        <v>168070.5</v>
       </c>
       <c r="I24" s="18">
-        <f t="shared" si="2"/>
-        <v>15903338.75</v>
+        <f t="shared" si="4"/>
+        <v>2435374.5</v>
       </c>
       <c r="J24" s="18">
-        <f>SUM(J17:J23)</f>
-        <v>552955</v>
+        <f t="shared" ref="J24:S39" si="6">SUM(J17:J23)</f>
+        <v>139729.20000000001</v>
       </c>
       <c r="K24" s="18">
-        <f>SUM(K17:K23)</f>
-        <v>423540</v>
+        <f t="shared" si="6"/>
+        <v>200366.40000000002</v>
       </c>
       <c r="L24" s="18">
-        <f>SUM(L17:L23)</f>
-        <v>238241.25</v>
+        <f t="shared" si="6"/>
+        <v>53387.100000000006</v>
       </c>
       <c r="M24" s="18">
-        <f>SUM(M17:M23)</f>
-        <v>1214736.25</v>
+        <f>SUM(J24:L24)</f>
+        <v>393482.70000000007</v>
       </c>
       <c r="N24" s="18">
-        <f>SUM(N17:N23)</f>
-        <v>970612.5</v>
+        <f t="shared" si="6"/>
+        <v>217503.00000000003</v>
       </c>
       <c r="O24" s="18">
-        <f>SUM(O17:O23)</f>
-        <v>423540</v>
+        <f t="shared" si="6"/>
+        <v>94910.399999999994</v>
       </c>
       <c r="P24" s="18">
-        <f>SUM(P17:P23)</f>
-        <v>1411800</v>
+        <f t="shared" si="6"/>
+        <v>316368</v>
       </c>
       <c r="Q24" s="18">
-        <f>SUM(Q17:Q23)</f>
-        <v>926493.75</v>
+        <f t="shared" si="6"/>
+        <v>207616.50000000003</v>
       </c>
       <c r="R24" s="18">
-        <f>SUM(R17:R23)</f>
-        <v>58825</v>
+        <f t="shared" si="6"/>
+        <v>13182</v>
       </c>
       <c r="S24" s="20">
-        <f>SUM(S17:S23)</f>
-        <v>3791271.25</v>
+        <f>SUM(N24:R24)</f>
+        <v>849579.9</v>
       </c>
       <c r="T24" s="21">
-        <f t="shared" si="3"/>
-        <v>17118075</v>
+        <f>SUM(I24+M24)</f>
+        <v>2828857.2</v>
       </c>
       <c r="V24" s="5">
-        <f t="shared" ref="V24:AJ24" si="4">SUM(V17:V23)</f>
-        <v>10906.125</v>
+        <f t="shared" ref="V24:AJ24" si="7">SUM(V17:V23)</f>
+        <v>3375.0300000000007</v>
       </c>
       <c r="W24" s="5">
-        <f t="shared" si="4"/>
-        <v>10782.5625</v>
+        <f t="shared" si="7"/>
+        <v>4278.4349999999995</v>
       </c>
       <c r="X24" s="5">
-        <f t="shared" si="4"/>
-        <v>7617.8125</v>
+        <f t="shared" si="7"/>
+        <v>2482.9749999999999</v>
       </c>
       <c r="Y24" s="5">
-        <f t="shared" si="4"/>
-        <v>7151.9375</v>
+        <f t="shared" si="7"/>
+        <v>1788.8850000000002</v>
       </c>
       <c r="Z24" s="5">
-        <f t="shared" si="4"/>
-        <v>12752.0625</v>
+        <f t="shared" si="7"/>
+        <v>3509.3550000000005</v>
       </c>
       <c r="AA24" s="5">
-        <f t="shared" si="4"/>
-        <v>4290.6875</v>
+        <f t="shared" si="7"/>
+        <v>1209.7850000000001</v>
       </c>
       <c r="AB24" s="5">
-        <f t="shared" si="4"/>
-        <v>7982.5</v>
+        <f t="shared" si="7"/>
+        <v>3418.2</v>
       </c>
       <c r="AC24" s="5">
-        <f t="shared" si="4"/>
-        <v>11282.625</v>
+        <f t="shared" si="7"/>
+        <v>2838.6700000000005</v>
       </c>
       <c r="AD24" s="5">
-        <f t="shared" si="4"/>
-        <v>7335.4375</v>
+        <f t="shared" si="7"/>
+        <v>2885.2449999999999</v>
       </c>
       <c r="AE24" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF24" s="5">
-        <f t="shared" si="4"/>
-        <v>1322.375</v>
+        <f t="shared" si="7"/>
+        <v>637.73</v>
       </c>
       <c r="AG24" s="5">
-        <f t="shared" si="4"/>
-        <v>4170.6875</v>
+        <f t="shared" si="7"/>
+        <v>1089.7850000000001</v>
       </c>
       <c r="AH24" s="5">
-        <f t="shared" si="4"/>
-        <v>5494.25</v>
+        <f t="shared" si="7"/>
+        <v>1386.38</v>
       </c>
       <c r="AI24" s="5">
-        <f t="shared" si="4"/>
-        <v>91089.0625</v>
+        <f t="shared" si="7"/>
+        <v>28900.475000000002</v>
       </c>
       <c r="AJ24" s="8">
-        <f t="shared" si="4"/>
-        <v>17209164.0625</v>
+        <f t="shared" si="7"/>
+        <v>2857757.6750000003</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.55000000000000004">
@@ -1886,30 +1892,42 @@
       </c>
       <c r="B25" s="11">
         <f>B32*0.3</f>
-        <v>821535</v>
+        <v>976950</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="19">
-        <f>$K6 * (B25*B12)</f>
-        <v>18073.77</v>
-      </c>
+      <c r="F25" s="19"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="18"/>
+      <c r="H25" s="19">
+        <f>$M6 * (B25*B12)</f>
+        <v>97695</v>
+      </c>
+      <c r="I25" s="18">
+        <f t="shared" si="4"/>
+        <v>97695</v>
+      </c>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
-      <c r="M25" s="18"/>
+      <c r="M25" s="18">
+        <f t="shared" ref="M25:M40" si="8">SUM(J25:L25)</f>
+        <v>0</v>
+      </c>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="20"/>
+      <c r="R25" s="19">
+        <f>$H6 * (B25*B12)</f>
+        <v>97695</v>
+      </c>
+      <c r="S25" s="20">
+        <f t="shared" ref="S25:S40" si="9">SUM(N25:R25)</f>
+        <v>97695</v>
+      </c>
       <c r="T25" s="21"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
@@ -1918,7 +1936,7 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="7">
         <f>F6*2+(B25*0.7)</f>
-        <v>575714.5</v>
+        <v>684505</v>
       </c>
       <c r="AB25" s="7"/>
       <c r="AC25" s="7"/>
@@ -1928,56 +1946,65 @@
       <c r="AG25" s="7"/>
       <c r="AH25" s="7"/>
       <c r="AI25" s="5">
-        <f t="shared" ref="AI25:AI31" si="5">SUM(V25:AH25)</f>
-        <v>575714.5</v>
+        <f t="shared" ref="AI25:AI31" si="10">SUM(V25:AH25)</f>
+        <v>684505</v>
       </c>
       <c r="AJ25" s="8">
-        <f t="shared" ref="AJ25:AJ31" si="6">I25+M25+AI25</f>
-        <v>575714.5</v>
+        <f t="shared" ref="AJ25:AJ31" si="11">I25+M25+AI25</f>
+        <v>782200</v>
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2"/>
       <c r="B26" s="11">
         <f>B32*0.27</f>
-        <v>739381.5</v>
+        <v>879255</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" s="19">
         <f>$B6 * (B26*B12)</f>
-        <v>44362.890000000007</v>
+        <v>1055106</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19">
         <f>$K6 * (B26*B12)</f>
-        <v>16266.393000000002</v>
+        <v>386872.2</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
-      <c r="I26" s="18"/>
+      <c r="I26" s="18">
+        <f t="shared" si="4"/>
+        <v>1441978.2</v>
+      </c>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="18"/>
+      <c r="M26" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N26" s="19"/>
       <c r="O26" s="19"/>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
-      <c r="S26" s="20"/>
+      <c r="S26" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T26" s="21"/>
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7">
         <f>C6*1+(B26*0.7)</f>
-        <v>517767.05</v>
+        <v>615678.5</v>
       </c>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7">
         <f>E6*1+(B26*0.7)</f>
-        <v>517687.05</v>
+        <v>615598.5</v>
       </c>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
@@ -1988,46 +2015,61 @@
       <c r="AG26" s="7"/>
       <c r="AH26" s="7"/>
       <c r="AI26" s="5">
-        <f t="shared" si="5"/>
-        <v>1035454.1</v>
+        <f t="shared" si="10"/>
+        <v>1231277</v>
       </c>
       <c r="AJ26" s="8">
-        <f t="shared" si="6"/>
-        <v>1035454.1</v>
+        <f t="shared" si="11"/>
+        <v>2673255.2000000002</v>
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
       <c r="B27" s="11">
         <f>B32*0.17</f>
-        <v>465536.50000000006</v>
+        <v>553605</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19">
         <f>$C6 * (B27*B12)</f>
-        <v>4655.3650000000007</v>
+        <v>110721</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
+      <c r="I27" s="18">
+        <f t="shared" si="4"/>
+        <v>110721</v>
+      </c>
+      <c r="J27" s="19">
+        <f>$D6 * (B27*B12)</f>
+        <v>44288.4</v>
+      </c>
       <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="18"/>
+      <c r="L27" s="19">
+        <f>$J6 * (B27*B12)</f>
+        <v>149473.35</v>
+      </c>
+      <c r="M27" s="18">
+        <f t="shared" si="8"/>
+        <v>193761.75</v>
+      </c>
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
       <c r="R27" s="19"/>
-      <c r="S27" s="20"/>
+      <c r="S27" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T27" s="21"/>
       <c r="V27" s="7">
         <f>A6*1+(B27*B12)</f>
-        <v>223.276825</v>
+        <v>753.60500000000002</v>
       </c>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
@@ -2040,44 +2082,62 @@
       <c r="AE27" s="7"/>
       <c r="AF27" s="7">
         <f>K6*1+(B27*0.7)</f>
-        <v>326315.55000000005</v>
+        <v>387963.5</v>
       </c>
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="5">
-        <f t="shared" si="5"/>
-        <v>326538.82682500005</v>
+        <f t="shared" si="10"/>
+        <v>388717.10499999998</v>
       </c>
       <c r="AJ27" s="8">
-        <f t="shared" si="6"/>
-        <v>326538.82682500005</v>
+        <f t="shared" si="11"/>
+        <v>693199.85499999998</v>
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2"/>
       <c r="B28" s="11">
         <f>B32*0.09</f>
-        <v>246460.5</v>
+        <v>293085</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="G28" s="19">
+        <f>$L6 * (B28*B12)</f>
+        <v>58616.999999999993</v>
+      </c>
       <c r="H28" s="19"/>
-      <c r="I28" s="18"/>
+      <c r="I28" s="18">
+        <f t="shared" si="4"/>
+        <v>58616.999999999993</v>
+      </c>
       <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="K28" s="19">
+        <f>$I6 * (B28*B12)</f>
+        <v>234467.99999999997</v>
+      </c>
       <c r="L28" s="19"/>
-      <c r="M28" s="18"/>
+      <c r="M28" s="18">
+        <f t="shared" si="8"/>
+        <v>234467.99999999997</v>
+      </c>
       <c r="N28" s="19"/>
       <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
+      <c r="P28" s="19">
+        <f>$F6 * (B28*B12)</f>
+        <v>93787.199999999997</v>
+      </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
-      <c r="S28" s="20"/>
+      <c r="S28" s="20">
+        <f t="shared" si="9"/>
+        <v>93787.199999999997</v>
+      </c>
       <c r="T28" s="21"/>
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
@@ -2087,7 +2147,7 @@
       <c r="AA28" s="7"/>
       <c r="AB28" s="7">
         <f>G6*1+(B28*0.7)</f>
-        <v>173222.34999999998</v>
+        <v>205859.5</v>
       </c>
       <c r="AC28" s="7"/>
       <c r="AD28" s="7"/>
@@ -2096,52 +2156,70 @@
       <c r="AG28" s="7"/>
       <c r="AH28" s="7"/>
       <c r="AI28" s="5">
-        <f t="shared" si="5"/>
-        <v>173222.34999999998</v>
+        <f t="shared" si="10"/>
+        <v>205859.5</v>
       </c>
       <c r="AJ28" s="8">
-        <f t="shared" si="6"/>
-        <v>173222.34999999998</v>
+        <f t="shared" si="11"/>
+        <v>498944.49999999994</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="11">
         <f>B32*0.07</f>
-        <v>191691.50000000003</v>
+        <v>227955.00000000003</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="19">
         <f>$B6 * (B29*B12)</f>
-        <v>11501.490000000003</v>
+        <v>273546.00000000006</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="19"/>
+      <c r="H29" s="19">
+        <f>$M6 * (B29*B12)</f>
+        <v>22795.500000000004</v>
+      </c>
+      <c r="I29" s="18">
+        <f t="shared" si="4"/>
+        <v>296341.50000000006</v>
+      </c>
+      <c r="J29" s="19">
+        <f>$D6 * (B29*B12)</f>
+        <v>18236.400000000001</v>
+      </c>
       <c r="K29" s="19"/>
       <c r="L29" s="19"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="19"/>
+      <c r="M29" s="18">
+        <f t="shared" si="8"/>
+        <v>18236.400000000001</v>
+      </c>
+      <c r="N29" s="19">
+        <f>$D6 * (B29*B12)</f>
+        <v>18236.400000000001</v>
+      </c>
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
       <c r="R29" s="19"/>
-      <c r="S29" s="20"/>
+      <c r="S29" s="20">
+        <f t="shared" si="9"/>
+        <v>18236.400000000001</v>
+      </c>
       <c r="T29" s="21"/>
       <c r="V29" s="7"/>
       <c r="W29" s="7">
         <f>B6*1+(B29*0.7)</f>
-        <v>135384.05000000002</v>
+        <v>160768.5</v>
       </c>
       <c r="X29" s="7"/>
       <c r="Y29" s="7">
         <f>D6*1+(B29*0.7)</f>
-        <v>134264.05000000002</v>
+        <v>159648.5</v>
       </c>
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
@@ -2153,39 +2231,63 @@
       <c r="AG29" s="7"/>
       <c r="AH29" s="7"/>
       <c r="AI29" s="5">
-        <f t="shared" si="5"/>
-        <v>269648.10000000003</v>
+        <f t="shared" si="10"/>
+        <v>320417</v>
       </c>
       <c r="AJ29" s="8">
-        <f t="shared" si="6"/>
-        <v>269648.10000000003</v>
+        <f t="shared" si="11"/>
+        <v>634994.90000000014</v>
       </c>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2"/>
       <c r="B30" s="11">
         <f>B32*0.06</f>
-        <v>164307</v>
+        <v>195390</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="F30" s="19">
+        <f>$K6 * (B30*B12)</f>
+        <v>85971.6</v>
+      </c>
       <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="19"/>
+      <c r="H30" s="19">
+        <f>$M6 * (B30*B12)</f>
+        <v>19539</v>
+      </c>
+      <c r="I30" s="18">
+        <f t="shared" si="4"/>
+        <v>105510.6</v>
+      </c>
+      <c r="J30" s="19">
+        <f>$D6 * (B30*B12)</f>
+        <v>15631.2</v>
+      </c>
       <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="18"/>
+      <c r="L30" s="19">
+        <f>$J6 * (B30*B12)</f>
+        <v>52755.3</v>
+      </c>
+      <c r="M30" s="18">
+        <f t="shared" si="8"/>
+        <v>68386.5</v>
+      </c>
       <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="O30" s="19">
+        <f>$E6 * (B30*B12)</f>
+        <v>23446.800000000003</v>
+      </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
       <c r="R30" s="19"/>
-      <c r="S30" s="20"/>
+      <c r="S30" s="20">
+        <f t="shared" si="9"/>
+        <v>23446.800000000003</v>
+      </c>
       <c r="T30" s="21"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
@@ -2193,12 +2295,12 @@
       <c r="Y30" s="7"/>
       <c r="Z30" s="7">
         <f>E6*1+(B30*0.7)</f>
-        <v>115134.9</v>
+        <v>136893</v>
       </c>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7">
         <f>G6*2+(B30*0.7)</f>
-        <v>116414.9</v>
+        <v>138173</v>
       </c>
       <c r="AC30" s="7"/>
       <c r="AD30" s="7"/>
@@ -2207,51 +2309,69 @@
       <c r="AG30" s="7"/>
       <c r="AH30" s="7">
         <f>M6*1+(B30*0.7)</f>
-        <v>115114.9</v>
+        <v>136873</v>
       </c>
       <c r="AI30" s="5">
-        <f t="shared" si="5"/>
-        <v>346664.69999999995</v>
+        <f t="shared" si="10"/>
+        <v>411939</v>
       </c>
       <c r="AJ30" s="8">
-        <f t="shared" si="6"/>
-        <v>346664.69999999995</v>
+        <f t="shared" si="11"/>
+        <v>585836.1</v>
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
       <c r="B31" s="11">
         <f>B32*0.04</f>
-        <v>109538</v>
+        <v>130260</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19">
         <f>$C6 * (B31*B12)</f>
-        <v>1095.3800000000001</v>
+        <v>26052</v>
       </c>
       <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="G31" s="19">
+        <f>$L6 * (B31*B12)</f>
+        <v>26052</v>
+      </c>
       <c r="H31" s="19"/>
-      <c r="I31" s="18"/>
+      <c r="I31" s="18">
+        <f t="shared" si="4"/>
+        <v>52104</v>
+      </c>
       <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="K31" s="19">
+        <f>$I6 * (B31*B12)</f>
+        <v>104208</v>
+      </c>
       <c r="L31" s="19"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="19"/>
+      <c r="M31" s="18">
+        <f t="shared" si="8"/>
+        <v>104208</v>
+      </c>
+      <c r="N31" s="19">
+        <f>$A6 * (B31*B12)</f>
+        <v>26052</v>
+      </c>
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>
-      <c r="S31" s="20"/>
+      <c r="S31" s="20">
+        <f t="shared" si="9"/>
+        <v>26052</v>
+      </c>
       <c r="T31" s="21"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7">
         <f>C6*1+(B31*0.7)</f>
-        <v>76876.599999999991</v>
+        <v>91382</v>
       </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
@@ -2264,99 +2384,123 @@
       <c r="AG31" s="7"/>
       <c r="AH31" s="7"/>
       <c r="AI31" s="5">
-        <f t="shared" si="5"/>
-        <v>76876.599999999991</v>
+        <f t="shared" si="10"/>
+        <v>91382</v>
       </c>
       <c r="AJ31" s="8">
-        <f t="shared" si="6"/>
-        <v>76876.599999999991</v>
+        <f t="shared" si="11"/>
+        <v>247694</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="9">
-        <f>4213000*B13</f>
-        <v>2738450</v>
+        <f>B10*B13</f>
+        <v>3256500</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="D32" s="18">
+        <f>SUM(D25:D31)</f>
+        <v>1328652</v>
+      </c>
+      <c r="E32" s="18">
+        <f t="shared" ref="E32:H32" si="12">SUM(E25:E31)</f>
+        <v>136773</v>
+      </c>
+      <c r="F32" s="18">
+        <f t="shared" si="12"/>
+        <v>472843.80000000005</v>
+      </c>
+      <c r="G32" s="18">
+        <f t="shared" si="12"/>
+        <v>84669</v>
+      </c>
+      <c r="H32" s="18">
+        <f t="shared" si="12"/>
+        <v>140029.5</v>
+      </c>
+      <c r="I32" s="18">
+        <f t="shared" si="4"/>
+        <v>2162967.2999999998</v>
+      </c>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
+      <c r="M32" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N32" s="18"/>
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="18"/>
-      <c r="S32" s="20"/>
+      <c r="S32" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T32" s="21"/>
       <c r="V32" s="5">
-        <f t="shared" ref="V32:AB32" si="7">SUM(V25:V31)</f>
-        <v>223.276825</v>
+        <f t="shared" ref="V32:AB32" si="13">SUM(V25:V31)</f>
+        <v>753.60500000000002</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" si="7"/>
-        <v>135384.05000000002</v>
+        <f t="shared" si="13"/>
+        <v>160768.5</v>
       </c>
       <c r="X32" s="5">
-        <f t="shared" si="7"/>
-        <v>594643.65</v>
+        <f t="shared" si="13"/>
+        <v>707060.5</v>
       </c>
       <c r="Y32" s="5">
-        <f t="shared" si="7"/>
-        <v>134264.05000000002</v>
+        <f t="shared" si="13"/>
+        <v>159648.5</v>
       </c>
       <c r="Z32" s="5">
-        <f t="shared" si="7"/>
-        <v>632821.94999999995</v>
+        <f t="shared" si="13"/>
+        <v>752491.5</v>
       </c>
       <c r="AA32" s="5">
-        <f t="shared" si="7"/>
-        <v>575714.5</v>
+        <f t="shared" si="13"/>
+        <v>684505</v>
       </c>
       <c r="AB32" s="5">
-        <f t="shared" si="7"/>
-        <v>289637.25</v>
+        <f t="shared" si="13"/>
+        <v>344032.5</v>
       </c>
       <c r="AC32" s="5">
-        <f t="shared" ref="AC32:AH32" si="8">SUM(AC25:AC31)</f>
+        <f t="shared" ref="AC32:AH32" si="14">SUM(AC25:AC31)</f>
         <v>0</v>
       </c>
       <c r="AD32" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AE32" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AF32" s="5">
-        <f t="shared" si="8"/>
-        <v>326315.55000000005</v>
+        <f t="shared" si="14"/>
+        <v>387963.5</v>
       </c>
       <c r="AG32" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AH32" s="5">
-        <f t="shared" si="8"/>
-        <v>115114.9</v>
+        <f t="shared" si="14"/>
+        <v>136873</v>
       </c>
       <c r="AI32" s="5">
         <f>SUM(AI25:AI31)</f>
-        <v>2804119.1768250004</v>
+        <v>3334096.605</v>
       </c>
       <c r="AJ32" s="8">
         <f>SUM(AJ25:AJ31)</f>
-        <v>2804119.1768250004</v>
+        <v>6116124.5549999997</v>
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.55000000000000004">
@@ -2365,46 +2509,55 @@
       </c>
       <c r="B33" s="11">
         <f>B40*0.3</f>
-        <v>2407275</v>
+        <v>959400</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
-      <c r="I33" s="18"/>
+      <c r="I33" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
-      <c r="M33" s="18"/>
+      <c r="M33" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
-      <c r="S33" s="20"/>
+      <c r="S33" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T33" s="21"/>
       <c r="V33" s="7">
         <f>A6*3+(B33*B12)</f>
-        <v>720.36374999999998</v>
+        <v>1559.4</v>
       </c>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7">
         <f>E6*2+(B33*0.7)</f>
-        <v>1685332.5</v>
+        <v>671820</v>
       </c>
       <c r="AA33" s="7">
         <f>F6*2+(B33*0.7)</f>
-        <v>1685732.5</v>
+        <v>672220</v>
       </c>
       <c r="AB33" s="7">
         <f>G6*1+(B33*0.7)</f>
-        <v>1685792.5</v>
+        <v>672280</v>
       </c>
       <c r="AC33" s="7"/>
       <c r="AD33" s="7"/>
@@ -2413,57 +2566,66 @@
       <c r="AG33" s="7"/>
       <c r="AH33" s="7">
         <f>M6*4+(B33*0.7)</f>
-        <v>1685492.5</v>
+        <v>671980</v>
       </c>
       <c r="AI33" s="5">
-        <f t="shared" ref="AI33:AI39" si="9">SUM(V33:AH33)</f>
-        <v>6743070.3637499996</v>
+        <f t="shared" ref="AI33:AI39" si="15">SUM(V33:AH33)</f>
+        <v>2689859.4</v>
       </c>
       <c r="AJ33" s="8">
-        <f t="shared" ref="AJ33:AJ39" si="10">SUM(I33+M33+AI33)</f>
-        <v>6743070.3637499996</v>
+        <f t="shared" ref="AJ33:AJ39" si="16">SUM(I33+M33+AI33)</f>
+        <v>2689859.4</v>
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
       <c r="B34" s="11">
         <f>B40*0.27</f>
-        <v>2166547.5</v>
+        <v>863460</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
-      <c r="I34" s="18"/>
+      <c r="I34" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
       <c r="L34" s="19"/>
-      <c r="M34" s="18"/>
+      <c r="M34" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
       <c r="R34" s="19"/>
-      <c r="S34" s="20"/>
+      <c r="S34" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T34" s="21"/>
       <c r="V34" s="7"/>
       <c r="W34" s="7">
         <f>B6*1+(B34*0.7)</f>
-        <v>1517783.25</v>
+        <v>605622</v>
       </c>
       <c r="X34" s="7">
         <f>C6*3+(B34*0.7)</f>
-        <v>1517183.25</v>
+        <v>605022</v>
       </c>
       <c r="Y34" s="7"/>
       <c r="Z34" s="7"/>
       <c r="AA34" s="7">
         <f>F6*1+(B34*0.7)</f>
-        <v>1516903.25</v>
+        <v>604742</v>
       </c>
       <c r="AB34" s="7"/>
       <c r="AC34" s="7"/>
@@ -2473,45 +2635,54 @@
       <c r="AG34" s="7"/>
       <c r="AH34" s="7"/>
       <c r="AI34" s="5">
-        <f t="shared" si="9"/>
-        <v>4551869.75</v>
+        <f t="shared" si="15"/>
+        <v>1815386</v>
       </c>
       <c r="AJ34" s="8">
-        <f t="shared" si="10"/>
-        <v>4551869.75</v>
+        <f t="shared" si="16"/>
+        <v>1815386</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
       <c r="B35" s="11">
         <f>B40*0.17</f>
-        <v>1364122.5</v>
+        <v>543660</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
-      <c r="I35" s="18"/>
+      <c r="I35" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
-      <c r="M35" s="18"/>
+      <c r="M35" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
-      <c r="S35" s="20"/>
+      <c r="S35" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T35" s="21"/>
       <c r="V35" s="7"/>
       <c r="W35" s="7"/>
       <c r="X35" s="7">
         <f>C6*1+(B35*0.7)</f>
-        <v>955085.74999999988</v>
+        <v>380762</v>
       </c>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
@@ -2521,62 +2692,71 @@
       <c r="AD35" s="7"/>
       <c r="AE35" s="7">
         <f>J6*1+(B35*0.7)</f>
-        <v>955155.74999999988</v>
+        <v>380832</v>
       </c>
       <c r="AF35" s="7"/>
       <c r="AG35" s="7"/>
       <c r="AH35" s="7"/>
       <c r="AI35" s="5">
-        <f t="shared" si="9"/>
-        <v>1910241.4999999998</v>
+        <f t="shared" si="15"/>
+        <v>761594</v>
       </c>
       <c r="AJ35" s="8">
-        <f t="shared" si="10"/>
-        <v>1910241.4999999998</v>
+        <f t="shared" si="16"/>
+        <v>761594</v>
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2"/>
       <c r="B36" s="11">
         <f>B40*0.09</f>
-        <v>722182.5</v>
+        <v>287820</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
-      <c r="I36" s="18"/>
+      <c r="I36" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J36" s="19"/>
       <c r="K36" s="19"/>
       <c r="L36" s="19"/>
-      <c r="M36" s="18"/>
+      <c r="M36" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
       <c r="R36" s="19"/>
-      <c r="S36" s="20"/>
+      <c r="S36" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T36" s="21"/>
       <c r="V36" s="7"/>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7">
         <f>D6*1+(B36*0.7)</f>
-        <v>505607.74999999994</v>
+        <v>201554</v>
       </c>
       <c r="Z36" s="7">
         <f>E6*1+(B36*0.7)</f>
-        <v>505647.74999999994</v>
+        <v>201594</v>
       </c>
       <c r="AA36" s="7"/>
       <c r="AB36" s="7"/>
       <c r="AC36" s="7">
         <f>H6*1+(B36*0.7)</f>
-        <v>505627.74999999994</v>
+        <v>201574</v>
       </c>
       <c r="AD36" s="7"/>
       <c r="AE36" s="7"/>
@@ -2584,54 +2764,63 @@
       <c r="AG36" s="7"/>
       <c r="AH36" s="7"/>
       <c r="AI36" s="5">
-        <f t="shared" si="9"/>
-        <v>1516883.2499999998</v>
+        <f t="shared" si="15"/>
+        <v>604722</v>
       </c>
       <c r="AJ36" s="8">
-        <f t="shared" si="10"/>
-        <v>1516883.2499999998</v>
+        <f t="shared" si="16"/>
+        <v>604722</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
       <c r="B37" s="11">
         <f>B40*0.07</f>
-        <v>561697.5</v>
+        <v>223860.00000000003</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
-      <c r="I37" s="18"/>
+      <c r="I37" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
       <c r="L37" s="19"/>
-      <c r="M37" s="18"/>
+      <c r="M37" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N37" s="19"/>
       <c r="O37" s="19"/>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
       <c r="R37" s="19"/>
-      <c r="S37" s="20"/>
+      <c r="S37" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T37" s="21"/>
       <c r="V37" s="7">
         <f>A6*1+(B37)</f>
-        <v>561897.5</v>
+        <v>224060.00000000003</v>
       </c>
       <c r="W37" s="7">
         <f>B6*1+(B37*0.7)</f>
-        <v>394388.25</v>
+        <v>157902</v>
       </c>
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7">
         <f>F6*1+(B37*0.7)</f>
-        <v>393508.25</v>
+        <v>157022</v>
       </c>
       <c r="AB37" s="7"/>
       <c r="AC37" s="7"/>
@@ -2641,46 +2830,55 @@
       <c r="AG37" s="7"/>
       <c r="AH37" s="7">
         <f>M6*1+(B37*0.7)</f>
-        <v>393288.25</v>
+        <v>156802</v>
       </c>
       <c r="AI37" s="5">
-        <f t="shared" si="9"/>
-        <v>1743082.25</v>
+        <f t="shared" si="15"/>
+        <v>695786</v>
       </c>
       <c r="AJ37" s="8">
-        <f t="shared" si="10"/>
-        <v>1743082.25</v>
+        <f t="shared" si="16"/>
+        <v>695786</v>
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
       <c r="B38" s="11">
         <f>B40*0.06</f>
-        <v>481455</v>
+        <v>191880</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
-      <c r="I38" s="18"/>
+      <c r="I38" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
       <c r="L38" s="19"/>
-      <c r="M38" s="18"/>
+      <c r="M38" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N38" s="19"/>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
       <c r="Q38" s="19"/>
       <c r="R38" s="19"/>
-      <c r="S38" s="20"/>
+      <c r="S38" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T38" s="21"/>
       <c r="V38" s="7">
         <f>A6*1+(B38*B12)</f>
-        <v>224.07275000000001</v>
+        <v>391.88</v>
       </c>
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
@@ -2689,51 +2887,60 @@
       <c r="AA38" s="7"/>
       <c r="AB38" s="7">
         <f>G6*1+(B38*0.7)</f>
-        <v>337718.5</v>
+        <v>135016</v>
       </c>
       <c r="AC38" s="7"/>
       <c r="AD38" s="7"/>
       <c r="AE38" s="7"/>
       <c r="AF38" s="7">
         <f>K6*1+(B38*0.7)</f>
-        <v>337458.5</v>
+        <v>134756</v>
       </c>
       <c r="AG38" s="7"/>
       <c r="AH38" s="7"/>
       <c r="AI38" s="5">
-        <f t="shared" si="9"/>
-        <v>675401.07275000005</v>
+        <f t="shared" si="15"/>
+        <v>270163.88</v>
       </c>
       <c r="AJ38" s="8">
-        <f t="shared" si="10"/>
-        <v>675401.07275000005</v>
+        <f t="shared" si="16"/>
+        <v>270163.88</v>
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2"/>
       <c r="B39" s="11">
         <f>B40*0.04</f>
-        <v>320970</v>
+        <v>127920</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
-      <c r="I39" s="18"/>
+      <c r="I39" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
-      <c r="M39" s="18"/>
+      <c r="M39" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N39" s="19"/>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
       <c r="R39" s="19"/>
-      <c r="S39" s="20"/>
+      <c r="S39" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T39" s="21"/>
       <c r="V39" s="7"/>
       <c r="W39" s="7"/>
@@ -2743,7 +2950,7 @@
       <c r="Y39" s="7"/>
       <c r="Z39" s="7">
         <f>E6*1+(B39*0.7)</f>
-        <v>224799</v>
+        <v>89664</v>
       </c>
       <c r="AA39" s="7"/>
       <c r="AB39" s="7"/>
@@ -2753,28 +2960,28 @@
       <c r="AF39" s="7"/>
       <c r="AG39" s="7">
         <f>L6*1+(B39*0.7)</f>
-        <v>224879</v>
+        <v>89744</v>
       </c>
       <c r="AH39" s="7">
         <f>M6*1+(B39*0.7)</f>
-        <v>224779</v>
+        <v>89644</v>
       </c>
       <c r="AI39" s="5">
-        <f t="shared" si="9"/>
-        <v>674458</v>
+        <f t="shared" si="15"/>
+        <v>269053</v>
       </c>
       <c r="AJ39" s="8">
-        <f t="shared" si="10"/>
-        <v>674458</v>
+        <f t="shared" si="16"/>
+        <v>269053</v>
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" s="9">
-        <f>12345000*B13</f>
-        <v>8024250</v>
+        <f>C10*B13</f>
+        <v>3198000</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="18"/>
@@ -2782,69 +2989,78 @@
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
+      <c r="I40" s="18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="J40" s="18"/>
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
+      <c r="M40" s="18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
       <c r="P40" s="18"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="18"/>
-      <c r="S40" s="20"/>
+      <c r="S40" s="20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="T40" s="21"/>
       <c r="V40" s="5">
         <f>SUM(V33:V39)</f>
-        <v>562841.93650000007</v>
+        <v>226011.28000000003</v>
       </c>
       <c r="W40" s="5">
-        <f t="shared" ref="W40:AH40" si="11">SUM(W33:W39)</f>
-        <v>1912171.5</v>
+        <f t="shared" ref="W40:AH40" si="17">SUM(W33:W39)</f>
+        <v>763524</v>
       </c>
       <c r="X40" s="5">
-        <f t="shared" si="11"/>
-        <v>2472270</v>
+        <f t="shared" si="17"/>
+        <v>985785</v>
       </c>
       <c r="Y40" s="5">
-        <f t="shared" si="11"/>
-        <v>505607.74999999994</v>
+        <f t="shared" si="17"/>
+        <v>201554</v>
       </c>
       <c r="Z40" s="5">
-        <f t="shared" si="11"/>
-        <v>2415779.25</v>
+        <f t="shared" si="17"/>
+        <v>963078</v>
       </c>
       <c r="AA40" s="5">
-        <f t="shared" si="11"/>
-        <v>3596144</v>
+        <f t="shared" si="17"/>
+        <v>1433984</v>
       </c>
       <c r="AB40" s="5">
-        <f t="shared" si="11"/>
-        <v>2023511</v>
+        <f t="shared" si="17"/>
+        <v>807296</v>
       </c>
       <c r="AC40" s="5">
-        <f t="shared" si="11"/>
-        <v>505627.74999999994</v>
+        <f t="shared" si="17"/>
+        <v>201574</v>
       </c>
       <c r="AD40" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AE40" s="5">
-        <f t="shared" si="11"/>
-        <v>955155.74999999988</v>
+        <f t="shared" si="17"/>
+        <v>380832</v>
       </c>
       <c r="AF40" s="5">
-        <f t="shared" si="11"/>
-        <v>337458.5</v>
+        <f t="shared" si="17"/>
+        <v>134756</v>
       </c>
       <c r="AG40" s="5">
         <f>SUM(AG33:AG39)</f>
-        <v>224879</v>
+        <v>89744</v>
       </c>
       <c r="AH40" s="5">
-        <f t="shared" si="11"/>
-        <v>2303559.75</v>
+        <f t="shared" si="17"/>
+        <v>918426</v>
       </c>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="8"/>
@@ -2853,101 +3069,119 @@
       <c r="A41" s="4"/>
       <c r="B41" s="10">
         <f>B24+B32+B40</f>
-        <v>304887700</v>
+        <v>9750000</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="21">
         <f>SUM(D24+D32+D40)</f>
-        <v>11294400</v>
+        <v>2673216</v>
       </c>
       <c r="E41" s="21">
         <f>SUM(E24+E32+E40)</f>
-        <v>617662.5</v>
+        <v>275184</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
       <c r="H41" s="21">
         <f>SUM(H24+H32+H40)</f>
-        <v>750018.75</v>
+        <v>308100</v>
       </c>
       <c r="I41" s="21">
         <f>SUM(I40+I32+I24)</f>
-        <v>15903338.75</v>
+        <v>4598341.8</v>
       </c>
       <c r="J41" s="21">
         <f>J24+J32+J40</f>
-        <v>552955</v>
+        <v>139729.20000000001</v>
       </c>
       <c r="K41" s="21">
-        <f t="shared" ref="K41:L41" si="12">K24+K32+K40</f>
-        <v>423540</v>
+        <f t="shared" ref="K41:L41" si="18">K24+K32+K40</f>
+        <v>200366.40000000002</v>
       </c>
       <c r="L41" s="21">
-        <f t="shared" si="12"/>
-        <v>238241.25</v>
+        <f>L24+L32+L40</f>
+        <v>53387.100000000006</v>
       </c>
       <c r="M41" s="21">
         <f>M24+M32+M40</f>
-        <v>1214736.25</v>
-      </c>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
+        <v>393482.70000000007</v>
+      </c>
+      <c r="N41" s="21">
+        <f>SUM(N24+N32+N40)</f>
+        <v>217503.00000000003</v>
+      </c>
+      <c r="O41" s="21">
+        <f t="shared" ref="O41:S41" si="19">SUM(O24+O32+O40)</f>
+        <v>94910.399999999994</v>
+      </c>
+      <c r="P41" s="21">
+        <f t="shared" si="19"/>
+        <v>316368</v>
+      </c>
+      <c r="Q41" s="21">
+        <f t="shared" si="19"/>
+        <v>207616.50000000003</v>
+      </c>
+      <c r="R41" s="21">
+        <f t="shared" si="19"/>
+        <v>13182</v>
+      </c>
+      <c r="S41" s="21">
+        <f t="shared" si="19"/>
+        <v>849579.9</v>
+      </c>
       <c r="T41" s="21"/>
       <c r="V41" s="8">
         <f>SUM(V24+V32+V40)</f>
-        <v>573971.33832500002</v>
+        <v>230139.91500000004</v>
       </c>
       <c r="W41" s="8">
-        <f t="shared" ref="W41:AH41" si="13">SUM(W24+W32+W40)</f>
-        <v>2058338.1125</v>
+        <f t="shared" ref="W41:AH41" si="20">SUM(W24+W32+W40)</f>
+        <v>928570.93500000006</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" si="13"/>
-        <v>3074531.4624999999</v>
+        <f t="shared" si="20"/>
+        <v>1695328.4750000001</v>
       </c>
       <c r="Y41" s="8">
-        <f t="shared" si="13"/>
-        <v>647023.73749999993</v>
+        <f t="shared" si="20"/>
+        <v>362991.38500000001</v>
       </c>
       <c r="Z41" s="8">
-        <f t="shared" si="13"/>
-        <v>3061353.2625000002</v>
+        <f t="shared" si="20"/>
+        <v>1719078.855</v>
       </c>
       <c r="AA41" s="8">
-        <f t="shared" si="13"/>
-        <v>4176149.1875</v>
+        <f t="shared" si="20"/>
+        <v>2119698.7850000001</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" si="13"/>
-        <v>2321130.75</v>
+        <f t="shared" si="20"/>
+        <v>1154746.7</v>
       </c>
       <c r="AC41" s="8">
-        <f t="shared" si="13"/>
-        <v>516910.37499999994</v>
+        <f t="shared" si="20"/>
+        <v>204412.67</v>
       </c>
       <c r="AD41" s="8">
-        <f t="shared" si="13"/>
-        <v>7335.4375</v>
+        <f t="shared" si="20"/>
+        <v>2885.2449999999999</v>
       </c>
       <c r="AE41" s="8">
-        <f t="shared" si="13"/>
-        <v>955155.74999999988</v>
+        <f t="shared" si="20"/>
+        <v>380832</v>
       </c>
       <c r="AF41" s="8">
-        <f t="shared" si="13"/>
-        <v>665096.42500000005</v>
+        <f t="shared" si="20"/>
+        <v>523357.23</v>
       </c>
       <c r="AG41" s="8">
-        <f t="shared" si="13"/>
-        <v>229049.6875</v>
+        <f t="shared" si="20"/>
+        <v>90833.785000000003</v>
       </c>
       <c r="AH41" s="8">
-        <f t="shared" si="13"/>
-        <v>2424168.9</v>
+        <f t="shared" si="20"/>
+        <v>1056685.3799999999</v>
       </c>
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>

</xml_diff>

<commit_message>
Edited excel capstone project.
Added all data needed to start adding it to PowerBI
</commit_message>
<xml_diff>
--- a/Capstone Project/Monika/Costs PerV3.xlsx
+++ b/Capstone Project/Monika/Costs PerV3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Desktop\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\Monika\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mszuc\Desktop\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\Monika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ABF808-1784-48D5-A2E4-CDC35919F222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC2B2C7-D272-461D-BF21-D9F794FB6F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{ED117939-1D2E-4498-B130-96B64592D033}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Seats And Restraints</t>
   </si>
@@ -156,6 +155,9 @@
   </si>
   <si>
     <t>% of Repairs</t>
+  </si>
+  <si>
+    <t>Accessories</t>
   </si>
 </sst>
 </file>
@@ -643,48 +645,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6105DF2C-7430-48BF-A45E-C623D48AA4A1}">
   <dimension ref="A2:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.89453125" customWidth="1"/>
-    <col min="2" max="2" width="21.68359375" customWidth="1"/>
-    <col min="3" max="3" width="15.7890625" customWidth="1"/>
-    <col min="4" max="4" width="18.3125" customWidth="1"/>
-    <col min="5" max="7" width="16.26171875" customWidth="1"/>
-    <col min="8" max="8" width="16.9453125" customWidth="1"/>
-    <col min="9" max="9" width="18.9453125" customWidth="1"/>
-    <col min="10" max="10" width="18.7890625" customWidth="1"/>
-    <col min="11" max="11" width="17.15625" customWidth="1"/>
-    <col min="12" max="12" width="19.15625" customWidth="1"/>
-    <col min="13" max="13" width="21.68359375" customWidth="1"/>
-    <col min="14" max="14" width="18.3125" customWidth="1"/>
-    <col min="15" max="21" width="12.734375" customWidth="1"/>
-    <col min="22" max="22" width="18.41796875" customWidth="1"/>
-    <col min="23" max="23" width="21.3125" customWidth="1"/>
-    <col min="24" max="24" width="19.734375" customWidth="1"/>
-    <col min="25" max="25" width="22.1015625" customWidth="1"/>
-    <col min="26" max="26" width="19.1015625" customWidth="1"/>
-    <col min="27" max="27" width="18.7890625" customWidth="1"/>
-    <col min="28" max="28" width="23.26171875" customWidth="1"/>
-    <col min="29" max="29" width="22.578125" customWidth="1"/>
-    <col min="30" max="31" width="19.7890625" customWidth="1"/>
-    <col min="32" max="32" width="20.3125" customWidth="1"/>
-    <col min="33" max="33" width="22.3125" customWidth="1"/>
-    <col min="34" max="34" width="21.9453125" customWidth="1"/>
-    <col min="35" max="35" width="15.7890625" customWidth="1"/>
-    <col min="36" max="36" width="18.05078125" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="7" width="16.265625" customWidth="1"/>
+    <col min="8" max="8" width="16.9296875" customWidth="1"/>
+    <col min="9" max="9" width="18.9296875" customWidth="1"/>
+    <col min="10" max="10" width="18.796875" customWidth="1"/>
+    <col min="11" max="11" width="17.1328125" customWidth="1"/>
+    <col min="12" max="12" width="19.1328125" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="21" width="12.73046875" customWidth="1"/>
+    <col min="22" max="22" width="18.3984375" customWidth="1"/>
+    <col min="23" max="23" width="21.33203125" customWidth="1"/>
+    <col min="24" max="24" width="19.73046875" customWidth="1"/>
+    <col min="25" max="25" width="22.06640625" customWidth="1"/>
+    <col min="26" max="26" width="19.06640625" customWidth="1"/>
+    <col min="27" max="27" width="18.796875" customWidth="1"/>
+    <col min="28" max="28" width="23.265625" customWidth="1"/>
+    <col min="29" max="29" width="22.59765625" customWidth="1"/>
+    <col min="30" max="31" width="19.796875" customWidth="1"/>
+    <col min="32" max="32" width="20.33203125" customWidth="1"/>
+    <col min="33" max="33" width="22.33203125" customWidth="1"/>
+    <col min="34" max="34" width="21.9296875" customWidth="1"/>
+    <col min="35" max="35" width="15.796875" customWidth="1"/>
+    <col min="36" max="36" width="18.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" ht="38.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:36" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="6"/>
       <c r="L3" s="7"/>
@@ -701,7 +703,7 @@
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
@@ -717,7 +719,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
         <v>15</v>
       </c>
@@ -769,7 +771,7 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23">
         <v>200</v>
       </c>
@@ -821,7 +823,7 @@
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -847,7 +849,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="28" t="s">
         <v>38</v>
       </c>
@@ -875,7 +877,7 @@
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
     </row>
-    <row r="9" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="27">
         <v>2019</v>
       </c>
@@ -907,7 +909,7 @@
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
     </row>
-    <row r="10" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:36" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="29">
         <v>5070000</v>
       </c>
@@ -939,7 +941,7 @@
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
     </row>
-    <row r="11" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
@@ -965,7 +967,7 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:36" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="24" t="s">
         <v>40</v>
       </c>
@@ -995,7 +997,7 @@
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="24" t="s">
         <v>39</v>
       </c>
@@ -1016,7 +1018,7 @@
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1063,7 +1065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>31</v>
@@ -1168,7 +1170,7 @@
       </c>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>2019</v>
       </c>
@@ -1181,44 +1183,47 @@
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="17">
-        <f>$K6 * (B17*B12)</f>
-        <v>435006</v>
-      </c>
+      <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
-        <f>$M6 * (B17*B12)</f>
-        <v>98865</v>
+        <f>$B6 * (B17*B12)</f>
+        <v>1186380</v>
       </c>
       <c r="I17" s="18">
         <f>SUM(D17:H17)</f>
-        <v>533871</v>
-      </c>
-      <c r="J17" s="17">
-        <f>$D6 * (B17*B12)</f>
-        <v>79092</v>
-      </c>
-      <c r="K17" s="19"/>
+        <v>1186380</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="19">
+        <f>$B6 * (B17*B12)</f>
+        <v>1186380</v>
+      </c>
       <c r="L17" s="19"/>
       <c r="M17" s="18">
         <f t="shared" ref="M17:M23" si="0">SUM(J17:L17)</f>
-        <v>79092</v>
-      </c>
-      <c r="N17" s="19"/>
+        <v>1186380</v>
+      </c>
+      <c r="N17" s="19">
+        <f>$B6 * (B17*B12)</f>
+        <v>1186380</v>
+      </c>
       <c r="O17" s="19"/>
-      <c r="P17" s="19">
-        <f>$F6 * (B17*B12)</f>
-        <v>316368</v>
-      </c>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19">
+        <f>$B6 * (B17*B12)</f>
+        <v>1186380</v>
+      </c>
+      <c r="R17" s="19">
+        <f>$B6 * (B17*B12)</f>
+        <v>1186380</v>
+      </c>
       <c r="S17" s="20">
         <f t="shared" ref="S17:S23" si="1">SUM(N17:R17)</f>
-        <v>316368</v>
+        <v>3559140</v>
       </c>
       <c r="T17" s="21">
         <f>SUM(I17+M17)</f>
-        <v>612963</v>
+        <v>2372760</v>
       </c>
       <c r="V17" s="7">
         <f>A$6*4+(B17*B12)</f>
@@ -1263,10 +1268,10 @@
       </c>
       <c r="AJ17" s="8">
         <f t="shared" ref="AJ17:AJ23" si="3">SUM(I17+M17+AI17)</f>
-        <v>624992.19999999995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>2384789.2000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
       <c r="B18" s="11">
         <f>B24*0.27</f>
@@ -1275,11 +1280,11 @@
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17">
         <f>$B6 * (B18*B12)</f>
         <v>1067742</v>
       </c>
-      <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="I18" s="18">
@@ -1288,29 +1293,29 @@
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="19">
-        <f>$D6 * (B18*B12)</f>
-        <v>71182.8</v>
+        <f>$B6 * (B18*B12)</f>
+        <v>1067742</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="18">
         <f t="shared" si="0"/>
-        <v>71182.8</v>
-      </c>
-      <c r="N18" s="19">
-        <f>$A6 * (B18*B12)</f>
-        <v>177957.00000000003</v>
-      </c>
+        <v>1067742</v>
+      </c>
+      <c r="N18" s="19"/>
       <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="19">
+        <f>$B6 * (B18*B12)</f>
+        <v>1067742</v>
+      </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="19"/>
       <c r="S18" s="20">
         <f t="shared" si="1"/>
-        <v>177957.00000000003</v>
+        <v>1067742</v>
       </c>
       <c r="T18" s="21">
-        <f t="shared" ref="T18:T24" si="5">SUM(I18+M18)</f>
-        <v>1138924.8</v>
+        <f t="shared" ref="T18:T23" si="5">SUM(I18+M18)</f>
+        <v>2135484</v>
       </c>
       <c r="V18" s="7">
         <f>A$6*1+(B18*B12)</f>
@@ -1352,10 +1357,10 @@
       </c>
       <c r="AJ18" s="8">
         <f t="shared" si="3"/>
-        <v>1148113.2950000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>2144672.4950000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="11">
         <f>B24*0.17</f>
@@ -1365,45 +1370,45 @@
         <v>23</v>
       </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="17">
-        <f>$C6 * (B19*B12)</f>
-        <v>112047</v>
-      </c>
+      <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17">
-        <f>$M6 * (B19*B12)</f>
-        <v>56023.5</v>
-      </c>
+      <c r="G19" s="17">
+        <f>$B6 * (B19*B12)</f>
+        <v>672282</v>
+      </c>
+      <c r="H19" s="17"/>
       <c r="I19" s="18">
         <f t="shared" si="4"/>
-        <v>168070.5</v>
+        <v>672282</v>
       </c>
       <c r="J19" s="19">
-        <f>$D6 * (B19*B12)</f>
-        <v>44818.8</v>
+        <f>$B6 * (B19*B12)</f>
+        <v>672282</v>
       </c>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18">
         <f t="shared" si="0"/>
-        <v>44818.8</v>
+        <v>672282</v>
       </c>
       <c r="N19" s="19"/>
       <c r="O19" s="19">
-        <f>$E6 * (B19*B12)</f>
-        <v>67228.2</v>
+        <f>$B6 * (B19*B12)</f>
+        <v>672282</v>
       </c>
       <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
+      <c r="Q19" s="19">
+        <f>$B6 * (B19*B12)</f>
+        <v>672282</v>
+      </c>
       <c r="R19" s="19"/>
       <c r="S19" s="20">
         <f t="shared" si="1"/>
-        <v>67228.2</v>
+        <v>1344564</v>
       </c>
       <c r="T19" s="21">
         <f t="shared" si="5"/>
-        <v>212889.3</v>
+        <v>1344564</v>
       </c>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
@@ -1433,10 +1438,10 @@
       </c>
       <c r="AJ19" s="8">
         <f t="shared" si="3"/>
-        <v>214970.00499999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>1346644.7050000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="11">
         <f>B24*0.09</f>
@@ -1446,42 +1451,57 @@
         <v>24</v>
       </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="17">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
       <c r="F20" s="17">
-        <f>$K6 * (B20*B12)</f>
-        <v>130501.80000000002</v>
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="17">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
       <c r="I20" s="18">
         <f t="shared" si="4"/>
-        <v>130501.80000000002</v>
+        <v>1067742.0000000002</v>
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="19">
-        <f>$D6 * (B20*B12)</f>
-        <v>23727.600000000002</v>
-      </c>
-      <c r="L20" s="19"/>
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
+      <c r="L20" s="19">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
       <c r="M20" s="18">
         <f t="shared" si="0"/>
-        <v>23727.600000000002</v>
+        <v>711828.00000000012</v>
       </c>
       <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19">
-        <f>$G6 * (B20*B12)</f>
-        <v>207616.50000000003</v>
-      </c>
-      <c r="R20" s="19"/>
+      <c r="O20" s="19">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
+      <c r="P20" s="19">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19">
+        <f>$B6 * (B20*B12)</f>
+        <v>355914.00000000006</v>
+      </c>
       <c r="S20" s="20">
         <f t="shared" si="1"/>
-        <v>207616.50000000003</v>
+        <v>1067742.0000000002</v>
       </c>
       <c r="T20" s="21">
         <f t="shared" si="5"/>
-        <v>154229.40000000002</v>
+        <v>1779570.0000000005</v>
       </c>
       <c r="V20" s="7">
         <f>A6*1+(B20*B12)</f>
@@ -1514,10 +1534,10 @@
       </c>
       <c r="AJ20" s="8">
         <f t="shared" si="3"/>
-        <v>157315.78000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>1782656.3800000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="11">
         <f>B24*0.07</f>
@@ -1530,39 +1550,48 @@
         <f>$B6 * (B21*B12)</f>
         <v>276822.00000000006</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="17">
+        <f>$B6 * (B21*B12)</f>
+        <v>276822.00000000006</v>
+      </c>
       <c r="F21" s="17"/>
-      <c r="G21" s="17">
-        <f>$L6 * (B20*B12)</f>
-        <v>59319.000000000007</v>
-      </c>
-      <c r="H21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17">
+        <f>$B6 * (B21*B12)</f>
+        <v>276822.00000000006</v>
+      </c>
       <c r="I21" s="18">
         <f t="shared" si="4"/>
-        <v>336141.00000000006</v>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+        <v>830466.00000000023</v>
+      </c>
+      <c r="J21" s="19">
+        <f>$B6 * (B21*B12)</f>
+        <v>276822.00000000006</v>
+      </c>
+      <c r="K21" s="19">
+        <f>$B6 * (B21*B12)</f>
+        <v>276822.00000000006</v>
+      </c>
       <c r="L21" s="19"/>
       <c r="M21" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>553644.00000000012</v>
       </c>
       <c r="N21" s="19"/>
       <c r="O21" s="19">
-        <f>$E6 * (B21*B12)</f>
-        <v>27682.200000000004</v>
+        <f>$B6 * (B21*B12)</f>
+        <v>276822.00000000006</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
       <c r="S21" s="20">
         <f t="shared" si="1"/>
-        <v>27682.200000000004</v>
+        <v>276822.00000000006</v>
       </c>
       <c r="T21" s="21">
         <f t="shared" si="5"/>
-        <v>336141.00000000006</v>
+        <v>1384110.0000000005</v>
       </c>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
@@ -1586,10 +1615,10 @@
       </c>
       <c r="AJ21" s="8">
         <f t="shared" si="3"/>
-        <v>336491.68500000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>1384460.6850000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="11">
         <f>B24*0.06</f>
@@ -1602,30 +1631,30 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17">
-        <f>$K6 * (B21*B12)</f>
-        <v>101501.40000000001</v>
+        <f>$B6 * (B22*B12)</f>
+        <v>237276.00000000003</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="18">
         <f t="shared" si="4"/>
-        <v>101501.40000000001</v>
-      </c>
-      <c r="J22" s="19">
-        <f>$D6 * (B22*B12)</f>
-        <v>15818.400000000001</v>
-      </c>
-      <c r="K22" s="19"/>
+        <v>237276.00000000003</v>
+      </c>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19">
+        <f>$B6 * (B22*B12)</f>
+        <v>237276.00000000003</v>
+      </c>
       <c r="L22" s="19">
-        <f>$J6 * (B22*B12)</f>
-        <v>53387.100000000006</v>
+        <f>$B6 * (B22*B12)</f>
+        <v>237276.00000000003</v>
       </c>
       <c r="M22" s="18">
         <f t="shared" si="0"/>
-        <v>69205.5</v>
+        <v>474552.00000000006</v>
       </c>
       <c r="N22" s="19">
-        <f>$A6 * (B22*B12)</f>
-        <v>39546</v>
+        <f>$B6 * (B22*B12)</f>
+        <v>237276.00000000003</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="19"/>
@@ -1633,11 +1662,11 @@
       <c r="R22" s="19"/>
       <c r="S22" s="20">
         <f t="shared" si="1"/>
-        <v>39546</v>
+        <v>237276.00000000003</v>
       </c>
       <c r="T22" s="21">
         <f t="shared" si="5"/>
-        <v>170706.90000000002</v>
+        <v>711828.00000000012</v>
       </c>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
@@ -1667,10 +1696,10 @@
       </c>
       <c r="AJ22" s="8">
         <f t="shared" si="3"/>
-        <v>172040.09000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>713161.19000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="11">
         <f>B24*0.04</f>
@@ -1681,47 +1710,50 @@
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17">
-        <f>$C6 * (B23*B12)</f>
-        <v>26364</v>
-      </c>
-      <c r="F23" s="17">
-        <f>$K6 * (B23*B12)</f>
-        <v>58000.799999999996</v>
-      </c>
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
+      </c>
+      <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
-        <f>$M6 * (B23*B12)</f>
-        <v>13182</v>
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
       </c>
       <c r="I23" s="18">
         <f>SUM(D23:H23)</f>
-        <v>97546.799999999988</v>
+        <v>316368</v>
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="19">
-        <f>$I6 * (B23*B12)</f>
-        <v>105456</v>
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
       </c>
       <c r="L23" s="19"/>
       <c r="M23" s="18">
         <f t="shared" si="0"/>
-        <v>105456</v>
+        <v>158184</v>
       </c>
       <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
+      <c r="O23" s="19">
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
+      </c>
+      <c r="P23" s="19">
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
+      </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="19">
-        <f>$H6 * (B23*B12)</f>
-        <v>13182</v>
+        <f>$B6 * (B23*B12)</f>
+        <v>158184</v>
       </c>
       <c r="S23" s="20">
         <f t="shared" si="1"/>
-        <v>13182</v>
+        <v>474552</v>
       </c>
       <c r="T23" s="21">
         <f t="shared" si="5"/>
-        <v>203002.8</v>
+        <v>474552</v>
       </c>
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
@@ -1745,10 +1777,10 @@
       </c>
       <c r="AJ23" s="8">
         <f t="shared" si="3"/>
-        <v>203834.62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>475383.82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -1759,71 +1791,71 @@
       <c r="C24" s="3"/>
       <c r="D24" s="18">
         <f>SUM(D17:D23)</f>
-        <v>1344564</v>
+        <v>276822.00000000006</v>
       </c>
       <c r="E24" s="18">
         <f>SUM(E17:E23)</f>
-        <v>138411</v>
+        <v>1858662</v>
       </c>
       <c r="F24" s="18">
         <f>SUM(F17:F23)</f>
-        <v>623508.60000000009</v>
+        <v>355914.00000000006</v>
       </c>
       <c r="G24" s="18">
         <f>SUM(G17:G23)</f>
-        <v>160820.40000000002</v>
+        <v>909558</v>
       </c>
       <c r="H24" s="18">
         <f>SUM(H17:H23)</f>
-        <v>168070.5</v>
+        <v>1977300</v>
       </c>
       <c r="I24" s="18">
-        <f t="shared" si="4"/>
-        <v>2435374.5</v>
+        <f>SUM(I17:I23)</f>
+        <v>5378256</v>
       </c>
       <c r="J24" s="18">
-        <f t="shared" ref="J24:S39" si="6">SUM(J17:J23)</f>
-        <v>139729.20000000001</v>
+        <f t="shared" ref="J24:R24" si="6">SUM(J17:J23)</f>
+        <v>949104</v>
       </c>
       <c r="K24" s="18">
         <f t="shared" si="6"/>
-        <v>200366.40000000002</v>
+        <v>3282318</v>
       </c>
       <c r="L24" s="18">
         <f t="shared" si="6"/>
-        <v>53387.100000000006</v>
+        <v>593190.00000000012</v>
       </c>
       <c r="M24" s="18">
-        <f>SUM(J24:L24)</f>
-        <v>393482.70000000007</v>
+        <f>SUM(M17:M23)</f>
+        <v>4824612</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="6"/>
-        <v>217503.00000000003</v>
+        <v>1423656</v>
       </c>
       <c r="O24" s="18">
         <f t="shared" si="6"/>
-        <v>94910.399999999994</v>
+        <v>1463202</v>
       </c>
       <c r="P24" s="18">
         <f t="shared" si="6"/>
-        <v>316368</v>
+        <v>1581840</v>
       </c>
       <c r="Q24" s="18">
         <f t="shared" si="6"/>
-        <v>207616.50000000003</v>
+        <v>1858662</v>
       </c>
       <c r="R24" s="18">
         <f t="shared" si="6"/>
-        <v>13182</v>
+        <v>1700478</v>
       </c>
       <c r="S24" s="20">
-        <f>SUM(N24:R24)</f>
-        <v>849579.9</v>
+        <f>SUM(S17:S23)</f>
+        <v>8027838</v>
       </c>
       <c r="T24" s="21">
         <f>SUM(I24+M24)</f>
-        <v>2828857.2</v>
+        <v>10202868</v>
       </c>
       <c r="V24" s="5">
         <f t="shared" ref="V24:AJ24" si="7">SUM(V17:V23)</f>
@@ -1883,10 +1915,10 @@
       </c>
       <c r="AJ24" s="8">
         <f t="shared" si="7"/>
-        <v>2857757.6750000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>10231768.475000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>2018</v>
       </c>
@@ -1902,31 +1934,34 @@
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
       <c r="H25" s="19">
-        <f>$M6 * (B25*B12)</f>
-        <v>97695</v>
+        <f>$B6 * (B25*B12)</f>
+        <v>1172340</v>
       </c>
       <c r="I25" s="18">
         <f t="shared" si="4"/>
-        <v>97695</v>
+        <v>1172340</v>
       </c>
       <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="K25" s="19">
+        <f>$B6 * (B25*B12)</f>
+        <v>1172340</v>
+      </c>
       <c r="L25" s="19"/>
       <c r="M25" s="18">
         <f t="shared" ref="M25:M40" si="8">SUM(J25:L25)</f>
-        <v>0</v>
+        <v>1172340</v>
       </c>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
       <c r="R25" s="19">
-        <f>$H6 * (B25*B12)</f>
-        <v>97695</v>
+        <f>$B6 * (B25*B12)</f>
+        <v>1172340</v>
       </c>
       <c r="S25" s="20">
         <f t="shared" ref="S25:S40" si="9">SUM(N25:R25)</f>
-        <v>97695</v>
+        <v>1172340</v>
       </c>
       <c r="T25" s="21"/>
       <c r="V25" s="7"/>
@@ -1951,10 +1986,10 @@
       </c>
       <c r="AJ25" s="8">
         <f t="shared" ref="AJ25:AJ31" si="11">I25+M25+AI25</f>
-        <v>782200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>3029185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="11">
         <f>B32*0.27</f>
@@ -1963,36 +1998,48 @@
       <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19">
         <f>$B6 * (B26*B12)</f>
         <v>1055106</v>
       </c>
-      <c r="E26" s="19"/>
       <c r="F26" s="19">
-        <f>$K6 * (B26*B12)</f>
-        <v>386872.2</v>
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
       </c>
       <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="H26" s="19">
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
+      </c>
       <c r="I26" s="18">
         <f t="shared" si="4"/>
-        <v>1441978.2</v>
-      </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+        <v>3165318</v>
+      </c>
+      <c r="J26" s="19">
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
+      </c>
+      <c r="K26" s="19">
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
+      </c>
       <c r="L26" s="19"/>
       <c r="M26" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2110212</v>
       </c>
       <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
+      <c r="O26" s="19">
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
+      </c>
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
       <c r="R26" s="19"/>
       <c r="S26" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1055106</v>
       </c>
       <c r="T26" s="21"/>
       <c r="V26" s="7"/>
@@ -2020,10 +2067,10 @@
       </c>
       <c r="AJ26" s="8">
         <f t="shared" si="11"/>
-        <v>2673255.2000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>6506807</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="11">
         <f>B32*0.17</f>
@@ -2032,39 +2079,48 @@
       <c r="C27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19">
-        <f>$C6 * (B27*B12)</f>
-        <v>110721</v>
-      </c>
+      <c r="D27" s="19">
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
+      </c>
+      <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="H27" s="19">
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
+      </c>
       <c r="I27" s="18">
         <f t="shared" si="4"/>
-        <v>110721</v>
+        <v>1328652</v>
       </c>
       <c r="J27" s="19">
-        <f>$D6 * (B27*B12)</f>
-        <v>44288.4</v>
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19">
-        <f>$J6 * (B27*B12)</f>
-        <v>149473.35</v>
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
       </c>
       <c r="M27" s="18">
         <f t="shared" si="8"/>
-        <v>193761.75</v>
-      </c>
-      <c r="N27" s="19"/>
+        <v>1328652</v>
+      </c>
+      <c r="N27" s="19">
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
+      </c>
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
+      <c r="R27" s="19">
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
+      </c>
       <c r="S27" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1328652</v>
       </c>
       <c r="T27" s="21"/>
       <c r="V27" s="7">
@@ -2092,10 +2148,10 @@
       </c>
       <c r="AJ27" s="8">
         <f t="shared" si="11"/>
-        <v>693199.85499999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>3046021.105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="11">
         <f>B32*0.09</f>
@@ -2106,37 +2162,46 @@
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="19">
+        <f>$B6 * (B28*B12)</f>
+        <v>351702</v>
+      </c>
       <c r="G28" s="19">
-        <f>$L6 * (B28*B12)</f>
-        <v>58616.999999999993</v>
-      </c>
-      <c r="H28" s="19"/>
+        <f>$B6 * (B28*B12)</f>
+        <v>351702</v>
+      </c>
+      <c r="H28" s="19">
+        <f>$B6 * (B26*B12)</f>
+        <v>1055106</v>
+      </c>
       <c r="I28" s="18">
         <f t="shared" si="4"/>
-        <v>58616.999999999993</v>
+        <v>1758510</v>
       </c>
       <c r="J28" s="19"/>
       <c r="K28" s="19">
-        <f>$I6 * (B28*B12)</f>
-        <v>234467.99999999997</v>
+        <f>$B6 * (B27*B12)</f>
+        <v>664326</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="18">
         <f t="shared" si="8"/>
-        <v>234467.99999999997</v>
+        <v>664326</v>
       </c>
       <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="O28" s="19">
+        <f>$B6 * (B28*B12)</f>
+        <v>351702</v>
+      </c>
       <c r="P28" s="19">
-        <f>$F6 * (B28*B12)</f>
-        <v>93787.199999999997</v>
+        <f>$B6 * (B28*B12)</f>
+        <v>351702</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
       <c r="S28" s="20">
         <f t="shared" si="9"/>
-        <v>93787.199999999997</v>
+        <v>703404</v>
       </c>
       <c r="T28" s="21"/>
       <c r="V28" s="7"/>
@@ -2161,10 +2226,10 @@
       </c>
       <c r="AJ28" s="8">
         <f t="shared" si="11"/>
-        <v>498944.49999999994</v>
-      </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>2628695.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="11">
         <f>B32*0.07</f>
@@ -2173,42 +2238,45 @@
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="19"/>
+      <c r="E29" s="19">
         <f>$B6 * (B29*B12)</f>
         <v>273546.00000000006</v>
       </c>
-      <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="19">
-        <f>$M6 * (B29*B12)</f>
-        <v>22795.500000000004</v>
+        <f>$B6 * (B29*B12)</f>
+        <v>273546.00000000006</v>
       </c>
       <c r="I29" s="18">
         <f t="shared" si="4"/>
-        <v>296341.50000000006</v>
-      </c>
-      <c r="J29" s="19">
-        <f>$D6 * (B29*B12)</f>
-        <v>18236.400000000001</v>
-      </c>
-      <c r="K29" s="19"/>
+        <v>547092.00000000012</v>
+      </c>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19">
+        <f>$B6 * (B29*B12)</f>
+        <v>273546.00000000006</v>
+      </c>
       <c r="L29" s="19"/>
       <c r="M29" s="18">
         <f t="shared" si="8"/>
-        <v>18236.400000000001</v>
-      </c>
-      <c r="N29" s="19">
-        <f>$D6 * (B29*B12)</f>
-        <v>18236.400000000001</v>
-      </c>
-      <c r="O29" s="19"/>
+        <v>273546.00000000006</v>
+      </c>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19">
+        <f>$B6 * (B29*B12)</f>
+        <v>273546.00000000006</v>
+      </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
+      <c r="R29" s="19">
+        <f>$B6 * (B29*B12)</f>
+        <v>273546.00000000006</v>
+      </c>
       <c r="S29" s="20">
         <f t="shared" si="9"/>
-        <v>18236.400000000001</v>
+        <v>547092.00000000012</v>
       </c>
       <c r="T29" s="21"/>
       <c r="V29" s="7"/>
@@ -2236,10 +2304,10 @@
       </c>
       <c r="AJ29" s="8">
         <f t="shared" si="11"/>
-        <v>634994.90000000014</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>1141055.0000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="11">
         <f>B32*0.06</f>
@@ -2250,43 +2318,37 @@
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
-      <c r="F30" s="19">
-        <f>$K6 * (B30*B12)</f>
-        <v>85971.6</v>
-      </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19">
-        <f>$M6 * (B30*B12)</f>
-        <v>19539</v>
-      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19">
+        <f>$B6 * (B30*B12)</f>
+        <v>234468.00000000003</v>
+      </c>
+      <c r="H30" s="19"/>
       <c r="I30" s="18">
         <f t="shared" si="4"/>
-        <v>105510.6</v>
-      </c>
-      <c r="J30" s="19">
-        <f>$D6 * (B30*B12)</f>
-        <v>15631.2</v>
-      </c>
+        <v>234468.00000000003</v>
+      </c>
+      <c r="J30" s="19"/>
       <c r="K30" s="19"/>
       <c r="L30" s="19">
-        <f>$J6 * (B30*B12)</f>
-        <v>52755.3</v>
+        <f>$B6 * (B30*B12)</f>
+        <v>234468.00000000003</v>
       </c>
       <c r="M30" s="18">
         <f t="shared" si="8"/>
-        <v>68386.5</v>
+        <v>234468.00000000003</v>
       </c>
       <c r="N30" s="19"/>
-      <c r="O30" s="19">
-        <f>$E6 * (B30*B12)</f>
-        <v>23446.800000000003</v>
-      </c>
+      <c r="O30" s="19"/>
       <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
+      <c r="Q30" s="19">
+        <f>$B6 * (B30*B12)</f>
+        <v>234468.00000000003</v>
+      </c>
       <c r="R30" s="19"/>
       <c r="S30" s="20">
         <f t="shared" si="9"/>
-        <v>23446.800000000003</v>
+        <v>234468.00000000003</v>
       </c>
       <c r="T30" s="21"/>
       <c r="V30" s="7"/>
@@ -2317,10 +2379,10 @@
       </c>
       <c r="AJ30" s="8">
         <f t="shared" si="11"/>
-        <v>585836.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>880875</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="11">
         <f>B32*0.04</f>
@@ -2329,42 +2391,48 @@
       <c r="C31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19">
-        <f>$C6 * (B31*B12)</f>
-        <v>26052</v>
-      </c>
+      <c r="D31" s="19">
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
+      </c>
+      <c r="E31" s="19"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="19">
-        <f>$L6 * (B31*B12)</f>
-        <v>26052</v>
-      </c>
-      <c r="H31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19">
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
+      </c>
       <c r="I31" s="18">
         <f t="shared" si="4"/>
-        <v>52104</v>
+        <v>312624</v>
       </c>
       <c r="J31" s="19"/>
-      <c r="K31" s="19">
-        <f>$I6 * (B31*B12)</f>
-        <v>104208</v>
-      </c>
-      <c r="L31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19">
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
+      </c>
       <c r="M31" s="18">
         <f t="shared" si="8"/>
-        <v>104208</v>
+        <v>156312</v>
       </c>
       <c r="N31" s="19">
-        <f>$A6 * (B31*B12)</f>
-        <v>26052</v>
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
       </c>
       <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
+      <c r="P31" s="19">
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
+      </c>
       <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
+      <c r="R31" s="19">
+        <f>$B6 * (B31*B12)</f>
+        <v>156312</v>
+      </c>
       <c r="S31" s="20">
         <f t="shared" si="9"/>
-        <v>26052</v>
+        <v>468936</v>
       </c>
       <c r="T31" s="21"/>
       <c r="V31" s="7"/>
@@ -2389,10 +2457,10 @@
       </c>
       <c r="AJ31" s="8">
         <f t="shared" si="11"/>
-        <v>247694</v>
-      </c>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>560318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -2403,95 +2471,119 @@
       <c r="C32" s="3"/>
       <c r="D32" s="18">
         <f>SUM(D25:D31)</f>
-        <v>1328652</v>
+        <v>820638</v>
       </c>
       <c r="E32" s="18">
         <f t="shared" ref="E32:H32" si="12">SUM(E25:E31)</f>
-        <v>136773</v>
+        <v>1328652</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" si="12"/>
-        <v>472843.80000000005</v>
+        <v>1406808</v>
       </c>
       <c r="G32" s="18">
         <f t="shared" si="12"/>
-        <v>84669</v>
+        <v>586170</v>
       </c>
       <c r="H32" s="18">
         <f t="shared" si="12"/>
-        <v>140029.5</v>
+        <v>4376736</v>
       </c>
       <c r="I32" s="18">
-        <f t="shared" si="4"/>
-        <v>2162967.2999999998</v>
-      </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
+        <f>SUM(I25:I31)</f>
+        <v>8519004</v>
+      </c>
+      <c r="J32" s="18">
+        <f>SUM(J25:J31)</f>
+        <v>1719432</v>
+      </c>
+      <c r="K32" s="18">
+        <f>SUM(K25:K31)</f>
+        <v>3165318</v>
+      </c>
+      <c r="L32" s="18">
+        <f>SUM(L25:L31)</f>
+        <v>1055106</v>
+      </c>
       <c r="M32" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
+        <f>SUM(M25:M31)</f>
+        <v>5939856</v>
+      </c>
+      <c r="N32" s="18">
+        <f>SUM(N25:N31)</f>
+        <v>820638</v>
+      </c>
+      <c r="O32" s="18">
+        <f>SUM(O25:O31)</f>
+        <v>1680354</v>
+      </c>
+      <c r="P32" s="18">
+        <f t="shared" ref="P32:R32" si="13">SUM(P25:P31)</f>
+        <v>508014</v>
+      </c>
+      <c r="Q32" s="18">
+        <f t="shared" si="13"/>
+        <v>234468.00000000003</v>
+      </c>
+      <c r="R32" s="18">
+        <f>SUM(R25:R31)</f>
+        <v>2266524</v>
+      </c>
       <c r="S32" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>SUM(S25:S31)</f>
+        <v>5509998</v>
       </c>
       <c r="T32" s="21"/>
       <c r="V32" s="5">
-        <f t="shared" ref="V32:AB32" si="13">SUM(V25:V31)</f>
+        <f t="shared" ref="V32:AB32" si="14">SUM(V25:V31)</f>
         <v>753.60500000000002</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>160768.5</v>
       </c>
       <c r="X32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>707060.5</v>
       </c>
       <c r="Y32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>159648.5</v>
       </c>
       <c r="Z32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>752491.5</v>
       </c>
       <c r="AA32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>684505</v>
       </c>
       <c r="AB32" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>344032.5</v>
       </c>
       <c r="AC32" s="5">
-        <f t="shared" ref="AC32:AH32" si="14">SUM(AC25:AC31)</f>
+        <f t="shared" ref="AC32:AH32" si="15">SUM(AC25:AC31)</f>
         <v>0</v>
       </c>
       <c r="AD32" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AE32" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AF32" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>387963.5</v>
       </c>
       <c r="AG32" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AH32" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>136873</v>
       </c>
       <c r="AI32" s="5">
@@ -2500,10 +2592,10 @@
       </c>
       <c r="AJ32" s="8">
         <f>SUM(AJ25:AJ31)</f>
-        <v>6116124.5549999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <v>17792956.605</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>2017</v>
       </c>
@@ -2518,26 +2610,35 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="H33" s="19">
+        <f>$B6 * (B33*B12)</f>
+        <v>1151280</v>
+      </c>
       <c r="I33" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="19"/>
+        <v>1151280</v>
+      </c>
+      <c r="J33" s="19">
+        <f>$B6 * (B33*B12)</f>
+        <v>1151280</v>
+      </c>
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
       <c r="M33" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1151280</v>
       </c>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
       <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
+      <c r="R33" s="19">
+        <f>$B6 * (B33*B12)</f>
+        <v>1151280</v>
+      </c>
       <c r="S33" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1151280</v>
       </c>
       <c r="T33" s="21"/>
       <c r="V33" s="7">
@@ -2569,15 +2670,15 @@
         <v>671980</v>
       </c>
       <c r="AI33" s="5">
-        <f t="shared" ref="AI33:AI39" si="15">SUM(V33:AH33)</f>
+        <f t="shared" ref="AI33:AI39" si="16">SUM(V33:AH33)</f>
         <v>2689859.4</v>
       </c>
       <c r="AJ33" s="8">
-        <f t="shared" ref="AJ33:AJ39" si="16">SUM(I33+M33+AI33)</f>
-        <v>2689859.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="AJ33:AJ39" si="17">SUM(I33+M33+AI33)</f>
+        <v>4992419.4000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="11">
         <f>B40*0.27</f>
@@ -2586,30 +2687,51 @@
       <c r="C34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="G34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
+      <c r="H34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
       <c r="I34" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+        <v>3108456</v>
+      </c>
+      <c r="J34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
+      <c r="K34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
       <c r="L34" s="19"/>
       <c r="M34" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="19"/>
+        <v>2072304</v>
+      </c>
+      <c r="N34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
+      <c r="R34" s="19">
+        <f>$B6 * (B34*B12)</f>
+        <v>1036152</v>
+      </c>
       <c r="S34" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2072304</v>
       </c>
       <c r="T34" s="21"/>
       <c r="V34" s="7"/>
@@ -2635,15 +2757,15 @@
       <c r="AG34" s="7"/>
       <c r="AH34" s="7"/>
       <c r="AI34" s="5">
-        <f t="shared" si="15"/>
-        <v>1815386</v>
-      </c>
-      <c r="AJ34" s="8">
         <f t="shared" si="16"/>
         <v>1815386</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ34" s="8">
+        <f t="shared" si="17"/>
+        <v>6996146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A35" s="2"/>
       <c r="B35" s="11">
         <f>B40*0.17</f>
@@ -2653,29 +2775,47 @@
         <v>23</v>
       </c>
       <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
+      <c r="E35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="H35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="I35" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="19"/>
+        <v>1304784</v>
+      </c>
+      <c r="J35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
+      <c r="L35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="M35" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="19"/>
+        <v>1304784</v>
+      </c>
+      <c r="N35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
+      <c r="R35" s="19">
+        <f>$B6 * (B35*B12)</f>
+        <v>652392</v>
+      </c>
       <c r="S35" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1304784</v>
       </c>
       <c r="T35" s="21"/>
       <c r="V35" s="7"/>
@@ -2698,15 +2838,15 @@
       <c r="AG35" s="7"/>
       <c r="AH35" s="7"/>
       <c r="AI35" s="5">
-        <f t="shared" si="15"/>
-        <v>761594</v>
-      </c>
-      <c r="AJ35" s="8">
         <f t="shared" si="16"/>
         <v>761594</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ35" s="8">
+        <f t="shared" si="17"/>
+        <v>3371162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
       <c r="B36" s="11">
         <f>B40*0.09</f>
@@ -2715,30 +2855,54 @@
       <c r="C36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
       <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
+      <c r="F36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
+      <c r="G36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
+      <c r="H36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
       <c r="I36" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+        <v>1381536</v>
+      </c>
+      <c r="J36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
+      <c r="K36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
       <c r="L36" s="19"/>
       <c r="M36" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>690768</v>
       </c>
       <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
+      <c r="O36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
+      <c r="P36" s="19">
+        <f>$B6 * (B36*B12)</f>
+        <v>345384</v>
+      </c>
       <c r="Q36" s="19"/>
       <c r="R36" s="19"/>
       <c r="S36" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>690768</v>
       </c>
       <c r="T36" s="21"/>
       <c r="V36" s="7"/>
@@ -2764,15 +2928,15 @@
       <c r="AG36" s="7"/>
       <c r="AH36" s="7"/>
       <c r="AI36" s="5">
-        <f t="shared" si="15"/>
-        <v>604722</v>
-      </c>
-      <c r="AJ36" s="8">
         <f t="shared" si="16"/>
         <v>604722</v>
       </c>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ36" s="8">
+        <f t="shared" si="17"/>
+        <v>2677026</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A37" s="2"/>
       <c r="B37" s="11">
         <f>B40*0.07</f>
@@ -2782,29 +2946,44 @@
         <v>25</v>
       </c>
       <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
+      <c r="E37" s="19">
+        <f>$B6 * (B37*B12)</f>
+        <v>268632.00000000006</v>
+      </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
+      <c r="H37" s="19">
+        <f>$B6 * (B37*B12)</f>
+        <v>268632.00000000006</v>
+      </c>
       <c r="I37" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>537264.00000000012</v>
       </c>
       <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="K37" s="19">
+        <f>$B6 * (B37*B12)</f>
+        <v>268632.00000000006</v>
+      </c>
       <c r="L37" s="19"/>
       <c r="M37" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>268632.00000000006</v>
       </c>
       <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="O37" s="19">
+        <f>$B6 * (B37*B12)</f>
+        <v>268632.00000000006</v>
+      </c>
       <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
+      <c r="Q37" s="19">
+        <f>$B6 * (B37*B12)</f>
+        <v>268632.00000000006</v>
+      </c>
       <c r="R37" s="19"/>
       <c r="S37" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>537264.00000000012</v>
       </c>
       <c r="T37" s="21"/>
       <c r="V37" s="7">
@@ -2833,15 +3012,15 @@
         <v>156802</v>
       </c>
       <c r="AI37" s="5">
-        <f t="shared" si="15"/>
-        <v>695786</v>
-      </c>
-      <c r="AJ37" s="8">
         <f t="shared" si="16"/>
         <v>695786</v>
       </c>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ37" s="8">
+        <f t="shared" si="17"/>
+        <v>1501682.0000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
       <c r="B38" s="11">
         <f>B40*0.06</f>
@@ -2850,30 +3029,48 @@
       <c r="C38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19">
+        <f>$B6 * (B38*B12)</f>
+        <v>230256</v>
+      </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
+      <c r="G38" s="19">
+        <f>$B6 * (B38*B12)</f>
+        <v>230256</v>
+      </c>
       <c r="H38" s="19"/>
       <c r="I38" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="19"/>
+        <v>460512</v>
+      </c>
+      <c r="J38" s="19">
+        <f>$B6 * (B38*B12)</f>
+        <v>230256</v>
+      </c>
       <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
+      <c r="L38" s="19">
+        <f>$B6 * (B38*B12)</f>
+        <v>230256</v>
+      </c>
       <c r="M38" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>460512</v>
       </c>
       <c r="N38" s="19"/>
       <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
+      <c r="P38" s="19">
+        <f>$B6 * (B28*B12)</f>
+        <v>351702</v>
+      </c>
       <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
+      <c r="R38" s="19">
+        <f>$B6 * (B38*B12)</f>
+        <v>230256</v>
+      </c>
       <c r="S38" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>581958</v>
       </c>
       <c r="T38" s="21"/>
       <c r="V38" s="7">
@@ -2899,15 +3096,15 @@
       <c r="AG38" s="7"/>
       <c r="AH38" s="7"/>
       <c r="AI38" s="5">
-        <f t="shared" si="15"/>
-        <v>270163.88</v>
-      </c>
-      <c r="AJ38" s="8">
         <f t="shared" si="16"/>
         <v>270163.88</v>
       </c>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ38" s="8">
+        <f t="shared" si="17"/>
+        <v>1191187.8799999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A39" s="2"/>
       <c r="B39" s="11">
         <f>B40*0.04</f>
@@ -2918,28 +3115,43 @@
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="F39" s="19">
+        <f>$B6 * (B39*B12)</f>
+        <v>153504</v>
+      </c>
       <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="H39" s="19">
+        <f>$B6 * (B39*B12)</f>
+        <v>153504</v>
+      </c>
       <c r="I39" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="19"/>
+        <v>307008</v>
+      </c>
+      <c r="J39" s="19">
+        <f>$B6 * (B39*B12)</f>
+        <v>153504</v>
+      </c>
       <c r="K39" s="19"/>
       <c r="L39" s="19"/>
       <c r="M39" s="18">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N39" s="19"/>
+        <v>153504</v>
+      </c>
+      <c r="N39" s="19">
+        <f>$B6 * (B39*B12)</f>
+        <v>153504</v>
+      </c>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
+      <c r="R39" s="19">
+        <f>$B6 * (B39*B12)</f>
+        <v>153504</v>
+      </c>
       <c r="S39" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>307008</v>
       </c>
       <c r="T39" s="21"/>
       <c r="V39" s="7"/>
@@ -2967,15 +3179,15 @@
         <v>89644</v>
       </c>
       <c r="AI39" s="5">
-        <f t="shared" si="15"/>
-        <v>269053</v>
-      </c>
-      <c r="AJ39" s="8">
         <f t="shared" si="16"/>
         <v>269053</v>
       </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+      <c r="AJ39" s="8">
+        <f t="shared" si="17"/>
+        <v>729565</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>35</v>
       </c>
@@ -2984,30 +3196,69 @@
         <v>3198000</v>
       </c>
       <c r="C40" s="3"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="D40" s="18">
+        <f>SUM(D33:D39)</f>
+        <v>1611792</v>
+      </c>
+      <c r="E40" s="18">
+        <f>SUM(E33:E39)</f>
+        <v>921024</v>
+      </c>
+      <c r="F40" s="18">
+        <f>SUM(F33:F39)</f>
+        <v>498888</v>
+      </c>
+      <c r="G40" s="18">
+        <f>SUM(G33:G39)</f>
+        <v>1611792</v>
+      </c>
+      <c r="H40" s="18">
+        <f>SUM(H33:H39)</f>
+        <v>3607344</v>
+      </c>
       <c r="I40" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
+        <f>SUM(I33:I39)</f>
+        <v>8250840</v>
+      </c>
+      <c r="J40" s="18">
+        <f>SUM(J33:J39)</f>
+        <v>3568968</v>
+      </c>
+      <c r="K40" s="18">
+        <f>SUM(K33:K39)</f>
+        <v>1650168</v>
+      </c>
+      <c r="L40" s="18">
+        <f>SUM(L33:L39)</f>
+        <v>882648</v>
+      </c>
       <c r="M40" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
+        <f>SUM(M33:M39)</f>
+        <v>6101784</v>
+      </c>
+      <c r="N40" s="18">
+        <f>SUM(N33:N39)</f>
+        <v>1842048</v>
+      </c>
+      <c r="O40" s="18">
+        <f t="shared" ref="O40:R40" si="18">SUM(O33:O39)</f>
+        <v>614016</v>
+      </c>
+      <c r="P40" s="18">
+        <f t="shared" si="18"/>
+        <v>697086</v>
+      </c>
+      <c r="Q40" s="18">
+        <f t="shared" si="18"/>
+        <v>268632.00000000006</v>
+      </c>
+      <c r="R40" s="18">
+        <f>SUM(R33:R39)</f>
+        <v>3223584</v>
+      </c>
       <c r="S40" s="20">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>SUM(S33:S39)</f>
+        <v>6645366</v>
       </c>
       <c r="T40" s="21"/>
       <c r="V40" s="5">
@@ -3015,43 +3266,43 @@
         <v>226011.28000000003</v>
       </c>
       <c r="W40" s="5">
-        <f t="shared" ref="W40:AH40" si="17">SUM(W33:W39)</f>
+        <f t="shared" ref="W40:AH40" si="19">SUM(W33:W39)</f>
         <v>763524</v>
       </c>
       <c r="X40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>985785</v>
       </c>
       <c r="Y40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>201554</v>
       </c>
       <c r="Z40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>963078</v>
       </c>
       <c r="AA40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1433984</v>
       </c>
       <c r="AB40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>807296</v>
       </c>
       <c r="AC40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>201574</v>
       </c>
       <c r="AD40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>380832</v>
       </c>
       <c r="AF40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>134756</v>
       </c>
       <c r="AG40" s="5">
@@ -3059,13 +3310,13 @@
         <v>89744</v>
       </c>
       <c r="AH40" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>918426</v>
       </c>
       <c r="AI40" s="5"/>
       <c r="AJ40" s="8"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="10">
         <f>B24+B32+B40</f>
@@ -3074,61 +3325,67 @@
       <c r="C41" s="4"/>
       <c r="D41" s="21">
         <f>SUM(D24+D32+D40)</f>
-        <v>2673216</v>
+        <v>2709252</v>
       </c>
       <c r="E41" s="21">
         <f>SUM(E24+E32+E40)</f>
-        <v>275184</v>
-      </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+        <v>4108338</v>
+      </c>
+      <c r="F41" s="21">
+        <f>SUM(F24+F32+F40)</f>
+        <v>2261610</v>
+      </c>
+      <c r="G41" s="21">
+        <f>SUM(G24+G32+G40)</f>
+        <v>3107520</v>
+      </c>
       <c r="H41" s="21">
         <f>SUM(H24+H32+H40)</f>
-        <v>308100</v>
+        <v>9961380</v>
       </c>
       <c r="I41" s="21">
         <f>SUM(I40+I32+I24)</f>
-        <v>4598341.8</v>
+        <v>22148100</v>
       </c>
       <c r="J41" s="21">
         <f>J24+J32+J40</f>
-        <v>139729.20000000001</v>
+        <v>6237504</v>
       </c>
       <c r="K41" s="21">
-        <f t="shared" ref="K41:L41" si="18">K24+K32+K40</f>
-        <v>200366.40000000002</v>
+        <f t="shared" ref="K41" si="20">K24+K32+K40</f>
+        <v>8097804</v>
       </c>
       <c r="L41" s="21">
         <f>L24+L32+L40</f>
-        <v>53387.100000000006</v>
+        <v>2530944</v>
       </c>
       <c r="M41" s="21">
         <f>M24+M32+M40</f>
-        <v>393482.70000000007</v>
+        <v>16866252</v>
       </c>
       <c r="N41" s="21">
         <f>SUM(N24+N32+N40)</f>
-        <v>217503.00000000003</v>
+        <v>4086342</v>
       </c>
       <c r="O41" s="21">
-        <f t="shared" ref="O41:S41" si="19">SUM(O24+O32+O40)</f>
-        <v>94910.399999999994</v>
+        <f t="shared" ref="O41:S41" si="21">SUM(O24+O32+O40)</f>
+        <v>3757572</v>
       </c>
       <c r="P41" s="21">
-        <f t="shared" si="19"/>
-        <v>316368</v>
+        <f t="shared" si="21"/>
+        <v>2786940</v>
       </c>
       <c r="Q41" s="21">
-        <f t="shared" si="19"/>
-        <v>207616.50000000003</v>
+        <f t="shared" si="21"/>
+        <v>2361762</v>
       </c>
       <c r="R41" s="21">
-        <f t="shared" si="19"/>
-        <v>13182</v>
+        <f t="shared" si="21"/>
+        <v>7190586</v>
       </c>
       <c r="S41" s="21">
-        <f t="shared" si="19"/>
-        <v>849579.9</v>
+        <f>SUM(S24+S32+S40)</f>
+        <v>20183202</v>
       </c>
       <c r="T41" s="21"/>
       <c r="V41" s="8">
@@ -3136,62 +3393,62 @@
         <v>230139.91500000004</v>
       </c>
       <c r="W41" s="8">
-        <f t="shared" ref="W41:AH41" si="20">SUM(W24+W32+W40)</f>
+        <f t="shared" ref="W41:AH41" si="22">SUM(W24+W32+W40)</f>
         <v>928570.93500000006</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1695328.4750000001</v>
       </c>
       <c r="Y41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>362991.38500000001</v>
       </c>
       <c r="Z41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1719078.855</v>
       </c>
       <c r="AA41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2119698.7850000001</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1154746.7</v>
       </c>
       <c r="AC41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>204412.67</v>
       </c>
       <c r="AD41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2885.2449999999999</v>
       </c>
       <c r="AE41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>380832</v>
       </c>
       <c r="AF41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>523357.23</v>
       </c>
       <c r="AG41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>90833.785000000003</v>
       </c>
       <c r="AH41" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1056685.3799999999</v>
       </c>
       <c r="AI41" s="8"/>
       <c r="AJ41" s="8"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.45">
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>

</xml_diff>